<commit_message>
Update the 2025 Meet List
</commit_message>
<xml_diff>
--- a/2025/meet_list_data_ready.xlsx
+++ b/2025/meet_list_data_ready.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dburk\Documents\GitHub\sdxc-data\2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A6CC6B1-84F8-48E5-8B0D-E7DEB72412D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECA4E173-3CBD-4178-8FF6-DD2830A03305}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{1EB159B1-87E3-4E73-9839-0175057112CF}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="230">
   <si>
     <t>official_meet_name</t>
   </si>
@@ -83,33 +83,18 @@
     <t>winner</t>
   </si>
   <si>
-    <t>2023-08-25</t>
-  </si>
-  <si>
     <t>Don Ray Invitational</t>
   </si>
   <si>
     <t>deubrook</t>
   </si>
   <si>
-    <t>2023-08-26</t>
-  </si>
-  <si>
     <t>Mack Butler Invitational</t>
   </si>
   <si>
-    <t>Mobridge-Pollock XC Invitational</t>
-  </si>
-  <si>
-    <t>mobridge</t>
-  </si>
-  <si>
     <t>Milbank Breathe Easy</t>
   </si>
   <si>
-    <t>2023-08-28</t>
-  </si>
-  <si>
     <t>Mitchell Invitational</t>
   </si>
   <si>
@@ -122,15 +107,6 @@
     <t>dakota_valley</t>
   </si>
   <si>
-    <t>2023-08-29</t>
-  </si>
-  <si>
-    <t>Estelline Invite</t>
-  </si>
-  <si>
-    <t>estelline</t>
-  </si>
-  <si>
     <t>Gregory XC Invite</t>
   </si>
   <si>
@@ -155,18 +131,12 @@
     <t>redfield</t>
   </si>
   <si>
-    <t>2023-08-31</t>
-  </si>
-  <si>
     <t>Marlene Gustafson Ryan Day Invite</t>
   </si>
   <si>
     <t>faith</t>
   </si>
   <si>
-    <t>2023-09-01</t>
-  </si>
-  <si>
     <t>Augustana Twilight XC Meet</t>
   </si>
   <si>
@@ -179,9 +149,6 @@
     <t>spearfish</t>
   </si>
   <si>
-    <t>Red Cloud XC Meet</t>
-  </si>
-  <si>
     <t>redcloud</t>
   </si>
   <si>
@@ -191,9 +158,6 @@
     <t>canton</t>
   </si>
   <si>
-    <t>2023-09-05</t>
-  </si>
-  <si>
     <t>Jesse James XC Meet</t>
   </si>
   <si>
@@ -209,9 +173,6 @@
     <t>wessington281</t>
   </si>
   <si>
-    <t>2023-09-06</t>
-  </si>
-  <si>
     <t>Conference 281</t>
   </si>
   <si>
@@ -221,21 +182,12 @@
     <t>freeman_academy</t>
   </si>
   <si>
-    <t>Potter County Invitational</t>
-  </si>
-  <si>
-    <t>potter_county</t>
-  </si>
-  <si>
     <t>Belle Fourche Invitational</t>
   </si>
   <si>
     <t>belle</t>
   </si>
   <si>
-    <t>2023-09-07</t>
-  </si>
-  <si>
     <t>DeSmet Invite</t>
   </si>
   <si>
@@ -254,15 +206,9 @@
     <t>bennett_county</t>
   </si>
   <si>
-    <t>2023-09-08</t>
-  </si>
-  <si>
     <t>Heartland Preview</t>
   </si>
   <si>
-    <t>2023-09-09</t>
-  </si>
-  <si>
     <t>heartland_preview</t>
   </si>
   <si>
@@ -278,9 +224,6 @@
     <t>brandon</t>
   </si>
   <si>
-    <t>Milbank Grandstay Invitational</t>
-  </si>
-  <si>
     <t>milbank_grand_stay</t>
   </si>
   <si>
@@ -290,9 +233,6 @@
     <t>arlington</t>
   </si>
   <si>
-    <t>2023-09-11</t>
-  </si>
-  <si>
     <t>V-H/SLCC Meet</t>
   </si>
   <si>
@@ -311,21 +251,9 @@
     <t>webster</t>
   </si>
   <si>
-    <t>Charger Invitational XC Meet</t>
-  </si>
-  <si>
-    <t>sioux_falls_christian</t>
-  </si>
-  <si>
-    <t>2023-09-12</t>
-  </si>
-  <si>
     <t>Flyer Invite</t>
   </si>
   <si>
-    <t>2023-09-13</t>
-  </si>
-  <si>
     <t>freeman_flyer</t>
   </si>
   <si>
@@ -335,9 +263,6 @@
     <t>chamberlain</t>
   </si>
   <si>
-    <t>2023-09-14</t>
-  </si>
-  <si>
     <t>Eldon Knudson Invitational</t>
   </si>
   <si>
@@ -350,36 +275,21 @@
     <t>roncalli</t>
   </si>
   <si>
-    <t>Newwel Invitational</t>
-  </si>
-  <si>
     <t>newell</t>
   </si>
   <si>
-    <t>2023-09-15</t>
-  </si>
-  <si>
     <t>Battler Invitational</t>
   </si>
   <si>
     <t>gettysburg</t>
   </si>
   <si>
-    <t>2023-09-16</t>
-  </si>
-  <si>
     <t>Clyde Cotton XC Invite</t>
   </si>
   <si>
     <t>huron</t>
   </si>
   <si>
-    <t>Good Eagle Invitational</t>
-  </si>
-  <si>
-    <t>flandreau</t>
-  </si>
-  <si>
     <t>Lyman Raider Nation Inivtational</t>
   </si>
   <si>
@@ -392,9 +302,6 @@
     <t>alcester</t>
   </si>
   <si>
-    <t>2023-09-18</t>
-  </si>
-  <si>
     <t>Bon Homme XC Invite</t>
   </si>
   <si>
@@ -419,15 +326,9 @@
     <t>hot_springs</t>
   </si>
   <si>
-    <t>2023-09-19</t>
-  </si>
-  <si>
     <t>Cornbelt Conference</t>
   </si>
   <si>
-    <t>2023-09-20</t>
-  </si>
-  <si>
     <t>howard_cornbelt_conference</t>
   </si>
   <si>
@@ -443,9 +344,6 @@
     <t>plankinton</t>
   </si>
   <si>
-    <t>2023-09-21</t>
-  </si>
-  <si>
     <t>Brookings Russ Strande XC Invite</t>
   </si>
   <si>
@@ -476,21 +374,12 @@
     <t>rapid_city</t>
   </si>
   <si>
-    <t>2023-09-22</t>
-  </si>
-  <si>
     <t>Platte-Geddes Invite</t>
   </si>
   <si>
     <t>platte_geddes</t>
   </si>
   <si>
-    <t>2023-09-23</t>
-  </si>
-  <si>
-    <t>2023-09-25</t>
-  </si>
-  <si>
     <t>groton</t>
   </si>
   <si>
@@ -521,21 +410,12 @@
     <t>Jones County Invite</t>
   </si>
   <si>
-    <t>2023-09-26</t>
-  </si>
-  <si>
-    <t>2023-09-27</t>
-  </si>
-  <si>
     <t>sioux_valley</t>
   </si>
   <si>
     <t>todd_county</t>
   </si>
   <si>
-    <t>jones_county</t>
-  </si>
-  <si>
     <t>coleman_egan</t>
   </si>
   <si>
@@ -545,15 +425,9 @@
     <t>burke</t>
   </si>
   <si>
-    <t>2023-09-28</t>
-  </si>
-  <si>
     <t>Lennox XC Invite</t>
   </si>
   <si>
-    <t>Sisseton Invite</t>
-  </si>
-  <si>
     <t>Sturgis Invitational</t>
   </si>
   <si>
@@ -563,18 +437,12 @@
     <t>lennox</t>
   </si>
   <si>
-    <t>sisseton</t>
-  </si>
-  <si>
     <t>sturgis</t>
   </si>
   <si>
     <t>watertown</t>
   </si>
   <si>
-    <t>2023-09-30</t>
-  </si>
-  <si>
     <t>Action Club XC Meet</t>
   </si>
   <si>
@@ -590,9 +458,6 @@
     <t>ecc</t>
   </si>
   <si>
-    <t>2023-10-02</t>
-  </si>
-  <si>
     <t>Howard Invite</t>
   </si>
   <si>
@@ -605,9 +470,6 @@
     <t>SESD Conference</t>
   </si>
   <si>
-    <t>Tanager XC Invite</t>
-  </si>
-  <si>
     <t>howard</t>
   </si>
   <si>
@@ -617,12 +479,6 @@
     <t>sesd</t>
   </si>
   <si>
-    <t>vermillion</t>
-  </si>
-  <si>
-    <t>2023-10-03</t>
-  </si>
-  <si>
     <t>wall</t>
   </si>
   <si>
@@ -635,21 +491,12 @@
     <t>gettysburg_pre</t>
   </si>
   <si>
-    <t>2023-10-04</t>
-  </si>
-  <si>
-    <t>Dakota Valley Conference</t>
-  </si>
-  <si>
     <t>Lake Region Conference</t>
   </si>
   <si>
     <t>lake_region_conference</t>
   </si>
   <si>
-    <t>2023-10-05</t>
-  </si>
-  <si>
     <t>Big East Conference</t>
   </si>
   <si>
@@ -686,9 +533,6 @@
     <t>nec</t>
   </si>
   <si>
-    <t>2023-10-07</t>
-  </si>
-  <si>
     <t>ESD Conference</t>
   </si>
   <si>
@@ -704,9 +548,6 @@
     <t>best_west</t>
   </si>
   <si>
-    <t>2023-10-11</t>
-  </si>
-  <si>
     <t>SDHSAA Region 1A</t>
   </si>
   <si>
@@ -770,9 +611,6 @@
     <t>Metro Conference</t>
   </si>
   <si>
-    <t>2023-10-14</t>
-  </si>
-  <si>
     <t>metro_conference</t>
   </si>
   <si>
@@ -794,9 +632,6 @@
     <t>sdhsaa_aa</t>
   </si>
   <si>
-    <t>2023-10-21</t>
-  </si>
-  <si>
     <t>source</t>
   </si>
   <si>
@@ -809,12 +644,6 @@
     <t>white_river</t>
   </si>
   <si>
-    <t>Western Great Plains Conference</t>
-  </si>
-  <si>
-    <t>murdo_great_plains_conference</t>
-  </si>
-  <si>
     <t>mackbutler</t>
   </si>
   <si>
@@ -827,38 +656,83 @@
     <t>week</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>dakota_valley_conference</t>
+    <t>North Central Invitational</t>
+  </si>
+  <si>
+    <t>bowdle</t>
+  </si>
+  <si>
+    <t>Douglas Early Bird</t>
+  </si>
+  <si>
+    <t>douglas</t>
+  </si>
+  <si>
+    <t>Redhawk Run</t>
+  </si>
+  <si>
+    <t>hendricks</t>
+  </si>
+  <si>
+    <t>Mahpiya Luta Owayawa Invite</t>
+  </si>
+  <si>
+    <t>The Bank Invite</t>
+  </si>
+  <si>
+    <t>Hoven Greyhound Invitational</t>
+  </si>
+  <si>
+    <t>hoven</t>
+  </si>
+  <si>
+    <t>Britton-Hecla Invitational</t>
+  </si>
+  <si>
+    <t>britton</t>
+  </si>
+  <si>
+    <t>Newell Invitational</t>
+  </si>
+  <si>
+    <t>Humboldt XC Meet</t>
+  </si>
+  <si>
+    <t>humboldt</t>
+  </si>
+  <si>
+    <t>murdo</t>
+  </si>
+  <si>
+    <t>Castlewood Invite</t>
+  </si>
+  <si>
+    <t>castlewood</t>
+  </si>
+  <si>
+    <t>elk_point_huskies</t>
+  </si>
+  <si>
+    <t>EPJ Huskies Invitational</t>
+  </si>
+  <si>
+    <t>Irene-Wakonda Invite</t>
+  </si>
+  <si>
+    <t>irene</t>
+  </si>
+  <si>
+    <t>Roger Loecker XC Invite</t>
+  </si>
+  <si>
+    <t>huron_roger</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -868,6 +742,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -893,10 +775,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1231,19 +1125,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BABB3D95-ED19-41E8-9BC3-61C8F80036A4}">
-  <dimension ref="A1:G111"/>
+  <dimension ref="A1:G112"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomLeft" activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="29.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -1253,40 +1147,40 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>262</v>
+      <c r="D1" s="6" t="s">
+        <v>205</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>253</v>
+        <v>198</v>
       </c>
       <c r="G1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>263</v>
+      <c r="C2" s="3">
+        <v>45897</v>
+      </c>
+      <c r="D2" s="6">
+        <v>1</v>
       </c>
       <c r="E2">
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>254</v>
+        <v>199</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -1299,11 +1193,11 @@
       <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>263</v>
+      <c r="C3" s="3">
+        <v>45897</v>
+      </c>
+      <c r="D3" s="6">
+        <v>1</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -1314,22 +1208,19 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>263</v>
+        <v>204</v>
+      </c>
+      <c r="C4" s="3">
+        <v>45897</v>
+      </c>
+      <c r="D4" s="6">
+        <v>1</v>
       </c>
       <c r="E4">
         <v>0</v>
-      </c>
-      <c r="F4" t="s">
-        <v>254</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -1337,16 +1228,16 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>263</v>
+        <v>20</v>
+      </c>
+      <c r="C5" s="3">
+        <v>45897</v>
+      </c>
+      <c r="D5" s="6">
+        <v>1</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -1355,41 +1246,45 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>206</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>263</v>
+        <v>207</v>
+      </c>
+      <c r="C6" s="3">
+        <v>45897</v>
+      </c>
+      <c r="D6" s="6">
+        <v>1</v>
       </c>
       <c r="E6">
         <v>1</v>
       </c>
+      <c r="F6"/>
       <c r="G6">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="2">
+        <v>10</v>
+      </c>
+      <c r="C7" s="3">
+        <v>45897</v>
+      </c>
+      <c r="D7" s="6">
         <v>1</v>
       </c>
       <c r="E7">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="F7" t="s">
+        <v>199</v>
       </c>
       <c r="G7">
         <v>0</v>
@@ -1397,22 +1292,19 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>208</v>
       </c>
       <c r="B8" t="s">
-        <v>259</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>263</v>
+        <v>209</v>
+      </c>
+      <c r="C8" s="3">
+        <v>45898</v>
+      </c>
+      <c r="D8" s="6">
+        <v>1</v>
       </c>
       <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8" t="s">
-        <v>254</v>
+        <v>1</v>
       </c>
       <c r="G8">
         <v>0</v>
@@ -1420,19 +1312,22 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>263</v>
+        <v>202</v>
+      </c>
+      <c r="C9" s="3">
+        <v>45898</v>
+      </c>
+      <c r="D9" s="6">
+        <v>1</v>
       </c>
       <c r="E9">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="F9" t="s">
+        <v>199</v>
       </c>
       <c r="G9">
         <v>0</v>
@@ -1440,16 +1335,16 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>261</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>263</v>
+        <v>12</v>
+      </c>
+      <c r="C10" s="3">
+        <v>45898</v>
+      </c>
+      <c r="D10" s="6">
+        <v>1</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -1460,19 +1355,19 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>263</v>
+        <v>14</v>
+      </c>
+      <c r="C11" s="3">
+        <v>45898</v>
+      </c>
+      <c r="D11" s="6">
+        <v>1</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G11">
         <v>0</v>
@@ -1480,22 +1375,22 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B12" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>263</v>
+        <v>22</v>
+      </c>
+      <c r="C12" s="3">
+        <v>45902</v>
+      </c>
+      <c r="D12" s="6">
+        <v>1</v>
       </c>
       <c r="E12">
         <v>1</v>
       </c>
       <c r="F12" t="s">
-        <v>254</v>
+        <v>199</v>
       </c>
       <c r="G12">
         <v>0</v>
@@ -1503,16 +1398,16 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B13" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>263</v>
+        <v>24</v>
+      </c>
+      <c r="C13" s="3">
+        <v>45902</v>
+      </c>
+      <c r="D13" s="6">
+        <v>1</v>
       </c>
       <c r="E13">
         <v>1</v>
@@ -1523,19 +1418,22 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B14" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>263</v>
+        <v>26</v>
+      </c>
+      <c r="C14" s="3">
+        <v>45902</v>
+      </c>
+      <c r="D14" s="6">
+        <v>1</v>
       </c>
       <c r="E14">
         <v>1</v>
+      </c>
+      <c r="F14" t="s">
+        <v>199</v>
       </c>
       <c r="G14">
         <v>0</v>
@@ -1543,22 +1441,22 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B15" t="s">
-        <v>34</v>
-      </c>
-      <c r="C15" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>263</v>
+      <c r="C15" s="3">
+        <v>45902</v>
+      </c>
+      <c r="D15" s="6">
+        <v>1</v>
       </c>
       <c r="E15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F15" t="s">
-        <v>254</v>
+        <v>199</v>
       </c>
       <c r="G15">
         <v>0</v>
@@ -1566,22 +1464,19 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>35</v>
+        <v>210</v>
       </c>
       <c r="B16" t="s">
-        <v>36</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>263</v>
+        <v>211</v>
+      </c>
+      <c r="C16" s="3">
+        <v>45902</v>
+      </c>
+      <c r="D16" s="6">
+        <v>1</v>
       </c>
       <c r="E16">
-        <v>0</v>
-      </c>
-      <c r="F16" t="s">
-        <v>254</v>
+        <v>1</v>
       </c>
       <c r="G16">
         <v>0</v>
@@ -1589,16 +1484,16 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="B17" t="s">
-        <v>38</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>263</v>
+        <v>30</v>
+      </c>
+      <c r="C17" s="3">
+        <v>45904</v>
+      </c>
+      <c r="D17" s="6">
+        <v>1</v>
       </c>
       <c r="E17">
         <v>1</v>
@@ -1609,151 +1504,154 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="B18" t="s">
-        <v>41</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>263</v>
+        <v>34</v>
+      </c>
+      <c r="C18" s="3">
+        <v>45905</v>
+      </c>
+      <c r="D18" s="6">
+        <v>1</v>
       </c>
       <c r="E18">
         <v>1</v>
       </c>
+      <c r="F18" t="s">
+        <v>199</v>
+      </c>
       <c r="G18">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>43</v>
+        <v>212</v>
       </c>
       <c r="B19" t="s">
-        <v>44</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>263</v>
+        <v>37</v>
+      </c>
+      <c r="C19" s="3">
+        <v>45905</v>
+      </c>
+      <c r="D19" s="6">
+        <v>1</v>
       </c>
       <c r="E19">
         <v>1</v>
       </c>
       <c r="F19" t="s">
-        <v>254</v>
+        <v>199</v>
       </c>
       <c r="G19">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="B20" t="s">
-        <v>46</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>263</v>
+        <v>32</v>
+      </c>
+      <c r="C20" s="3">
+        <v>45905</v>
+      </c>
+      <c r="D20" s="6">
+        <v>1</v>
       </c>
       <c r="E20">
         <v>1</v>
       </c>
-      <c r="F20" t="s">
-        <v>254</v>
-      </c>
+      <c r="F20"/>
       <c r="G20">
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="B21" t="s">
-        <v>48</v>
-      </c>
-      <c r="C21" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" s="3">
+        <v>45905</v>
+      </c>
+      <c r="D21" s="6">
+        <v>1</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21" t="s">
+        <v>199</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22" s="4">
+        <v>45906</v>
+      </c>
+      <c r="D22" s="7">
+        <v>1</v>
+      </c>
+      <c r="E22" s="2">
+        <v>1</v>
+      </c>
+      <c r="F22" s="2"/>
+      <c r="G22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>42</v>
       </c>
-      <c r="D21" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="E21">
-        <v>1</v>
-      </c>
-      <c r="G21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>49</v>
-      </c>
-      <c r="B22" t="s">
-        <v>50</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="E22">
-        <v>1</v>
-      </c>
-      <c r="F22" t="s">
-        <v>254</v>
-      </c>
-      <c r="G22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>52</v>
-      </c>
       <c r="B23" t="s">
-        <v>53</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>264</v>
+        <v>43</v>
+      </c>
+      <c r="C23" s="3">
+        <v>45908</v>
+      </c>
+      <c r="D23" s="6">
+        <v>2</v>
       </c>
       <c r="E23">
         <v>1</v>
       </c>
-      <c r="F23" t="s">
-        <v>254</v>
-      </c>
+      <c r="F23"/>
       <c r="G23">
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="B24" t="s">
-        <v>55</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>264</v>
+        <v>41</v>
+      </c>
+      <c r="C24" s="3">
+        <v>45909</v>
+      </c>
+      <c r="D24" s="6">
+        <v>2</v>
       </c>
       <c r="E24">
         <v>1</v>
+      </c>
+      <c r="F24" t="s">
+        <v>199</v>
       </c>
       <c r="G24">
         <v>0</v>
@@ -1761,16 +1659,16 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>58</v>
+        <v>216</v>
       </c>
       <c r="B25" t="s">
-        <v>56</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>264</v>
+        <v>217</v>
+      </c>
+      <c r="C25" s="3">
+        <v>45909</v>
+      </c>
+      <c r="D25" s="6">
+        <v>2</v>
       </c>
       <c r="E25">
         <v>1</v>
@@ -1781,19 +1679,22 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>59</v>
+        <v>38</v>
       </c>
       <c r="B26" t="s">
-        <v>60</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>264</v>
+        <v>39</v>
+      </c>
+      <c r="C26" s="3">
+        <v>45909</v>
+      </c>
+      <c r="D26" s="6">
+        <v>2</v>
       </c>
       <c r="E26">
         <v>1</v>
+      </c>
+      <c r="F26" t="s">
+        <v>199</v>
       </c>
       <c r="G26">
         <v>0</v>
@@ -1801,42 +1702,39 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="B27" t="s">
-        <v>62</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>264</v>
+        <v>47</v>
+      </c>
+      <c r="C27" s="3">
+        <v>45910</v>
+      </c>
+      <c r="D27" s="6">
+        <v>2</v>
       </c>
       <c r="E27">
         <v>1</v>
       </c>
       <c r="G27">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>63</v>
+        <v>214</v>
       </c>
       <c r="B28" t="s">
-        <v>64</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>264</v>
+        <v>215</v>
+      </c>
+      <c r="C28" s="3">
+        <v>45910</v>
+      </c>
+      <c r="D28" s="6">
+        <v>2</v>
       </c>
       <c r="E28">
         <v>1</v>
-      </c>
-      <c r="F28" t="s">
-        <v>254</v>
       </c>
       <c r="G28">
         <v>0</v>
@@ -1844,19 +1742,22 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="B29" t="s">
-        <v>67</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>264</v>
+        <v>49</v>
+      </c>
+      <c r="C29" s="3">
+        <v>45911</v>
+      </c>
+      <c r="D29" s="6">
+        <v>2</v>
       </c>
       <c r="E29">
         <v>1</v>
+      </c>
+      <c r="F29" t="s">
+        <v>199</v>
       </c>
       <c r="G29">
         <v>0</v>
@@ -1864,42 +1765,39 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>68</v>
+        <v>50</v>
       </c>
       <c r="B30" t="s">
-        <v>69</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>264</v>
+        <v>51</v>
+      </c>
+      <c r="C30" s="3">
+        <v>45911</v>
+      </c>
+      <c r="D30" s="6">
+        <v>2</v>
       </c>
       <c r="E30">
         <v>1</v>
       </c>
       <c r="G30">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="B31" t="s">
-        <v>71</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>264</v>
+        <v>53</v>
+      </c>
+      <c r="C31" s="3">
+        <v>45911</v>
+      </c>
+      <c r="D31" s="6">
+        <v>2</v>
       </c>
       <c r="E31">
         <v>1</v>
-      </c>
-      <c r="F31" t="s">
-        <v>254</v>
       </c>
       <c r="G31">
         <v>0</v>
@@ -1907,19 +1805,22 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>73</v>
+        <v>54</v>
       </c>
       <c r="B32" t="s">
-        <v>75</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>264</v>
+        <v>55</v>
+      </c>
+      <c r="C32" s="3">
+        <v>45912</v>
+      </c>
+      <c r="D32" s="6">
+        <v>2</v>
       </c>
       <c r="E32">
         <v>1</v>
+      </c>
+      <c r="F32" t="s">
+        <v>199</v>
       </c>
       <c r="G32">
         <v>0</v>
@@ -1927,16 +1828,16 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>76</v>
+        <v>56</v>
       </c>
       <c r="B33" t="s">
-        <v>77</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>264</v>
+        <v>57</v>
+      </c>
+      <c r="C33" s="3">
+        <v>45913</v>
+      </c>
+      <c r="D33" s="6">
+        <v>2</v>
       </c>
       <c r="E33">
         <v>1</v>
@@ -1947,22 +1848,19 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="B34" t="s">
-        <v>79</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>264</v>
+        <v>59</v>
+      </c>
+      <c r="C34" s="3">
+        <v>45913</v>
+      </c>
+      <c r="D34" s="6">
+        <v>2</v>
       </c>
       <c r="E34">
         <v>1</v>
-      </c>
-      <c r="F34" t="s">
-        <v>254</v>
       </c>
       <c r="G34">
         <v>0</v>
@@ -1970,19 +1868,22 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="B35" t="s">
-        <v>81</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>264</v>
+        <v>61</v>
+      </c>
+      <c r="C35" s="3">
+        <v>45913</v>
+      </c>
+      <c r="D35" s="6">
+        <v>2</v>
       </c>
       <c r="E35">
         <v>1</v>
+      </c>
+      <c r="F35" t="s">
+        <v>199</v>
       </c>
       <c r="G35">
         <v>0</v>
@@ -1990,59 +1891,57 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>82</v>
+        <v>213</v>
       </c>
       <c r="B36" t="s">
-        <v>83</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>265</v>
+        <v>62</v>
+      </c>
+      <c r="C36" s="3">
+        <v>45913</v>
+      </c>
+      <c r="D36" s="6">
+        <v>2</v>
       </c>
       <c r="E36">
         <v>1</v>
       </c>
       <c r="G36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>255</v>
+        <v>63</v>
       </c>
       <c r="B37" t="s">
-        <v>256</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>265</v>
+        <v>64</v>
+      </c>
+      <c r="C37" s="3">
+        <v>45915</v>
+      </c>
+      <c r="D37" s="6">
+        <v>3</v>
       </c>
       <c r="E37">
         <v>1</v>
       </c>
-      <c r="F37" t="s">
-        <v>254</v>
-      </c>
+      <c r="F37"/>
       <c r="G37">
         <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="B38" t="s">
-        <v>86</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>265</v>
+        <v>66</v>
+      </c>
+      <c r="C38" s="3">
+        <v>45915</v>
+      </c>
+      <c r="D38" s="6">
+        <v>3</v>
       </c>
       <c r="E38">
         <v>1</v>
@@ -2053,36 +1952,36 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>87</v>
+        <v>67</v>
       </c>
       <c r="B39" t="s">
-        <v>88</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>265</v>
+        <v>68</v>
+      </c>
+      <c r="C39" s="3">
+        <v>45915</v>
+      </c>
+      <c r="D39" s="6">
+        <v>3</v>
       </c>
       <c r="E39">
         <v>1</v>
       </c>
       <c r="G39">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>89</v>
+        <v>69</v>
       </c>
       <c r="B40" t="s">
-        <v>90</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>265</v>
+        <v>70</v>
+      </c>
+      <c r="C40" s="3">
+        <v>45915</v>
+      </c>
+      <c r="D40" s="6">
+        <v>3</v>
       </c>
       <c r="E40">
         <v>1</v>
@@ -2093,22 +1992,22 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>91</v>
+        <v>200</v>
       </c>
       <c r="B41" t="s">
-        <v>92</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>265</v>
+        <v>201</v>
+      </c>
+      <c r="C41" s="3">
+        <v>45915</v>
+      </c>
+      <c r="D41" s="6">
+        <v>3</v>
       </c>
       <c r="E41">
         <v>1</v>
       </c>
       <c r="F41" t="s">
-        <v>254</v>
+        <v>199</v>
       </c>
       <c r="G41">
         <v>0</v>
@@ -2116,16 +2015,16 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>94</v>
+        <v>71</v>
       </c>
       <c r="B42" t="s">
-        <v>96</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>265</v>
+        <v>72</v>
+      </c>
+      <c r="C42" s="3">
+        <v>45917</v>
+      </c>
+      <c r="D42" s="6">
+        <v>3</v>
       </c>
       <c r="E42">
         <v>1</v>
@@ -2136,16 +2035,16 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B43" t="s">
-        <v>98</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>265</v>
+        <v>101</v>
+      </c>
+      <c r="C43" s="3">
+        <v>45917</v>
+      </c>
+      <c r="D43" s="6">
+        <v>3</v>
       </c>
       <c r="E43">
         <v>1</v>
@@ -2156,42 +2055,42 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>100</v>
+        <v>73</v>
       </c>
       <c r="B44" t="s">
-        <v>101</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>265</v>
+        <v>74</v>
+      </c>
+      <c r="C44" s="3">
+        <v>45918</v>
+      </c>
+      <c r="D44" s="6">
+        <v>3</v>
       </c>
       <c r="E44">
         <v>1</v>
       </c>
-      <c r="F44" t="s">
-        <v>254</v>
-      </c>
       <c r="G44">
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>102</v>
+        <v>75</v>
       </c>
       <c r="B45" t="s">
-        <v>103</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>265</v>
+        <v>76</v>
+      </c>
+      <c r="C45" s="3">
+        <v>45918</v>
+      </c>
+      <c r="D45" s="6">
+        <v>3</v>
       </c>
       <c r="E45">
         <v>1</v>
+      </c>
+      <c r="F45" t="s">
+        <v>199</v>
       </c>
       <c r="G45">
         <v>0</v>
@@ -2199,22 +2098,19 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>104</v>
+        <v>77</v>
       </c>
       <c r="B46" t="s">
-        <v>105</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>265</v>
+        <v>78</v>
+      </c>
+      <c r="C46" s="3">
+        <v>45918</v>
+      </c>
+      <c r="D46" s="6">
+        <v>3</v>
       </c>
       <c r="E46">
         <v>1</v>
-      </c>
-      <c r="F46" t="s">
-        <v>254</v>
       </c>
       <c r="G46">
         <v>0</v>
@@ -2222,42 +2118,42 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>107</v>
+        <v>218</v>
       </c>
       <c r="B47" t="s">
-        <v>108</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>265</v>
+        <v>79</v>
+      </c>
+      <c r="C47" s="3">
+        <v>45919</v>
+      </c>
+      <c r="D47" s="6">
+        <v>3</v>
       </c>
       <c r="E47">
         <v>1</v>
       </c>
+      <c r="F47" t="s">
+        <v>199</v>
+      </c>
       <c r="G47">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>110</v>
+        <v>80</v>
       </c>
       <c r="B48" t="s">
-        <v>111</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>265</v>
+        <v>81</v>
+      </c>
+      <c r="C48" s="3">
+        <v>45920</v>
+      </c>
+      <c r="D48" s="6">
+        <v>3</v>
       </c>
       <c r="E48">
         <v>1</v>
-      </c>
-      <c r="F48" t="s">
-        <v>254</v>
       </c>
       <c r="G48">
         <v>0</v>
@@ -2265,42 +2161,45 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>112</v>
+        <v>82</v>
       </c>
       <c r="B49" t="s">
-        <v>113</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>265</v>
+        <v>83</v>
+      </c>
+      <c r="C49" s="3">
+        <v>45920</v>
+      </c>
+      <c r="D49" s="6">
+        <v>3</v>
       </c>
       <c r="E49">
         <v>1</v>
       </c>
+      <c r="F49" t="s">
+        <v>199</v>
+      </c>
       <c r="G49">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>114</v>
+        <v>84</v>
       </c>
       <c r="B50" t="s">
-        <v>115</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="D50" s="2" t="s">
-        <v>265</v>
+        <v>85</v>
+      </c>
+      <c r="C50" s="3">
+        <v>45920</v>
+      </c>
+      <c r="D50" s="6">
+        <v>3</v>
       </c>
       <c r="E50">
         <v>1</v>
       </c>
       <c r="F50" t="s">
-        <v>254</v>
+        <v>199</v>
       </c>
       <c r="G50">
         <v>0</v>
@@ -2308,22 +2207,22 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>116</v>
+        <v>86</v>
       </c>
       <c r="B51" t="s">
-        <v>117</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>266</v>
+        <v>87</v>
+      </c>
+      <c r="C51" s="3">
+        <v>45922</v>
+      </c>
+      <c r="D51" s="6">
+        <v>4</v>
       </c>
       <c r="E51">
         <v>1</v>
       </c>
       <c r="F51" t="s">
-        <v>254</v>
+        <v>199</v>
       </c>
       <c r="G51">
         <v>0</v>
@@ -2331,42 +2230,42 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>119</v>
+        <v>88</v>
       </c>
       <c r="B52" t="s">
-        <v>120</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="D52" s="2" t="s">
-        <v>266</v>
+        <v>89</v>
+      </c>
+      <c r="C52" s="3">
+        <v>45922</v>
+      </c>
+      <c r="D52" s="6">
+        <v>4</v>
       </c>
       <c r="E52">
         <v>1</v>
       </c>
       <c r="G52">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>121</v>
+        <v>90</v>
       </c>
       <c r="B53" t="s">
-        <v>122</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>266</v>
+        <v>91</v>
+      </c>
+      <c r="C53" s="3">
+        <v>45922</v>
+      </c>
+      <c r="D53" s="6">
+        <v>4</v>
       </c>
       <c r="E53">
         <v>1</v>
       </c>
       <c r="F53" t="s">
-        <v>254</v>
+        <v>199</v>
       </c>
       <c r="G53">
         <v>0</v>
@@ -2374,16 +2273,16 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>123</v>
+        <v>92</v>
       </c>
       <c r="B54" t="s">
-        <v>124</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="D54" s="2" t="s">
-        <v>266</v>
+        <v>93</v>
+      </c>
+      <c r="C54" s="3">
+        <v>45922</v>
+      </c>
+      <c r="D54" s="6">
+        <v>4</v>
       </c>
       <c r="E54">
         <v>1</v>
@@ -2394,22 +2293,19 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>125</v>
+        <v>219</v>
       </c>
       <c r="B55" t="s">
-        <v>126</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>266</v>
+        <v>220</v>
+      </c>
+      <c r="C55" s="3">
+        <v>45922</v>
+      </c>
+      <c r="D55" s="6">
+        <v>4</v>
       </c>
       <c r="E55">
         <v>1</v>
-      </c>
-      <c r="F55" t="s">
-        <v>254</v>
       </c>
       <c r="G55">
         <v>0</v>
@@ -2417,56 +2313,60 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>128</v>
+        <v>94</v>
       </c>
       <c r="B56" t="s">
-        <v>130</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="D56" s="2" t="s">
-        <v>266</v>
+        <v>95</v>
+      </c>
+      <c r="C56" s="3">
+        <v>45923</v>
+      </c>
+      <c r="D56" s="6">
+        <v>4</v>
       </c>
       <c r="E56">
         <v>1</v>
       </c>
+      <c r="F56" t="s">
+        <v>199</v>
+      </c>
       <c r="G56">
         <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
-        <v>131</v>
-      </c>
-      <c r="B57" t="s">
-        <v>133</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="D57" s="2" t="s">
-        <v>266</v>
-      </c>
-      <c r="E57">
-        <v>1</v>
-      </c>
+      <c r="A57" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C57" s="4">
+        <v>45924</v>
+      </c>
+      <c r="D57" s="7">
+        <v>4</v>
+      </c>
+      <c r="E57" s="2">
+        <v>1</v>
+      </c>
+      <c r="F57" s="2"/>
       <c r="G57">
         <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>132</v>
+        <v>96</v>
       </c>
       <c r="B58" t="s">
-        <v>134</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="D58" s="2" t="s">
-        <v>266</v>
+        <v>97</v>
+      </c>
+      <c r="C58" s="3">
+        <v>45924</v>
+      </c>
+      <c r="D58" s="6">
+        <v>4</v>
       </c>
       <c r="E58">
         <v>1</v>
@@ -2477,22 +2377,22 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>257</v>
+        <v>123</v>
       </c>
       <c r="B59" t="s">
-        <v>258</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="D59" s="2" t="s">
-        <v>266</v>
+        <v>221</v>
+      </c>
+      <c r="C59" s="3">
+        <v>45924</v>
+      </c>
+      <c r="D59" s="6">
+        <v>4</v>
       </c>
       <c r="E59">
         <v>1</v>
       </c>
       <c r="F59" t="s">
-        <v>254</v>
+        <v>199</v>
       </c>
       <c r="G59">
         <v>0</v>
@@ -2500,22 +2400,19 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>136</v>
+        <v>98</v>
       </c>
       <c r="B60" t="s">
-        <v>140</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="D60" s="2" t="s">
-        <v>266</v>
+        <v>100</v>
+      </c>
+      <c r="C60" s="3">
+        <v>45924</v>
+      </c>
+      <c r="D60" s="6">
+        <v>4</v>
       </c>
       <c r="E60">
         <v>1</v>
-      </c>
-      <c r="F60" t="s">
-        <v>254</v>
       </c>
       <c r="G60">
         <v>0</v>
@@ -2523,19 +2420,22 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>137</v>
+        <v>102</v>
       </c>
       <c r="B61" t="s">
-        <v>141</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="D61" s="2" t="s">
-        <v>266</v>
+        <v>106</v>
+      </c>
+      <c r="C61" s="3">
+        <v>45925</v>
+      </c>
+      <c r="D61" s="6">
+        <v>4</v>
       </c>
       <c r="E61">
         <v>1</v>
+      </c>
+      <c r="F61" t="s">
+        <v>199</v>
       </c>
       <c r="G61">
         <v>0</v>
@@ -2543,42 +2443,42 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>138</v>
+        <v>103</v>
       </c>
       <c r="B62" t="s">
-        <v>143</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="D62" s="2" t="s">
-        <v>266</v>
+        <v>107</v>
+      </c>
+      <c r="C62" s="3">
+        <v>45925</v>
+      </c>
+      <c r="D62" s="6">
+        <v>4</v>
       </c>
       <c r="E62">
         <v>1</v>
       </c>
-      <c r="F62" t="s">
-        <v>254</v>
-      </c>
       <c r="G62">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>139</v>
+        <v>104</v>
       </c>
       <c r="B63" t="s">
-        <v>142</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="D63" s="2" t="s">
-        <v>266</v>
+        <v>109</v>
+      </c>
+      <c r="C63" s="3">
+        <v>45925</v>
+      </c>
+      <c r="D63" s="6">
+        <v>4</v>
       </c>
       <c r="E63">
         <v>1</v>
+      </c>
+      <c r="F63" t="s">
+        <v>199</v>
       </c>
       <c r="G63">
         <v>0</v>
@@ -2586,22 +2486,19 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>144</v>
+        <v>105</v>
       </c>
       <c r="B64" t="s">
-        <v>145</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="D64" s="2" t="s">
-        <v>266</v>
+        <v>108</v>
+      </c>
+      <c r="C64" s="3">
+        <v>45925</v>
+      </c>
+      <c r="D64" s="6">
+        <v>4</v>
       </c>
       <c r="E64">
         <v>1</v>
-      </c>
-      <c r="F64" t="s">
-        <v>254</v>
       </c>
       <c r="G64">
         <v>0</v>
@@ -2609,36 +2506,39 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>147</v>
+        <v>110</v>
       </c>
       <c r="B65" t="s">
-        <v>148</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="D65" s="2" t="s">
-        <v>266</v>
+        <v>111</v>
+      </c>
+      <c r="C65" s="3">
+        <v>45926</v>
+      </c>
+      <c r="D65" s="6">
+        <v>4</v>
       </c>
       <c r="E65">
         <v>1</v>
       </c>
+      <c r="F65" t="s">
+        <v>199</v>
+      </c>
       <c r="G65">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>154</v>
+        <v>222</v>
       </c>
       <c r="B66" t="s">
-        <v>151</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="D66" s="2" t="s">
-        <v>267</v>
+        <v>223</v>
+      </c>
+      <c r="C66" s="3">
+        <v>45927</v>
+      </c>
+      <c r="D66" s="6">
+        <v>4</v>
       </c>
       <c r="E66">
         <v>1</v>
@@ -2649,22 +2549,19 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>155</v>
+        <v>112</v>
       </c>
       <c r="B67" t="s">
-        <v>152</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="D67" s="2" t="s">
-        <v>267</v>
+        <v>113</v>
+      </c>
+      <c r="C67" s="3">
+        <v>45927</v>
+      </c>
+      <c r="D67" s="6">
+        <v>4</v>
       </c>
       <c r="E67">
         <v>1</v>
-      </c>
-      <c r="F67" t="s">
-        <v>254</v>
       </c>
       <c r="G67">
         <v>0</v>
@@ -2672,56 +2569,60 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>156</v>
+        <v>118</v>
       </c>
       <c r="B68" t="s">
-        <v>153</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="D68" s="2" t="s">
-        <v>267</v>
+        <v>115</v>
+      </c>
+      <c r="C68" s="3">
+        <v>45929</v>
+      </c>
+      <c r="D68" s="6">
+        <v>5</v>
       </c>
       <c r="E68">
         <v>1</v>
       </c>
+      <c r="F68" t="s">
+        <v>199</v>
+      </c>
       <c r="G68">
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>157</v>
+        <v>225</v>
       </c>
       <c r="B69" t="s">
-        <v>163</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="D69" s="2" t="s">
-        <v>267</v>
+        <v>224</v>
+      </c>
+      <c r="C69" s="3">
+        <v>45929</v>
+      </c>
+      <c r="D69" s="6">
+        <v>5</v>
       </c>
       <c r="E69">
         <v>1</v>
       </c>
+      <c r="F69"/>
       <c r="G69">
         <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>158</v>
+        <v>117</v>
       </c>
       <c r="B70" t="s">
-        <v>164</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="D70" s="2" t="s">
-        <v>267</v>
+        <v>114</v>
+      </c>
+      <c r="C70" s="3">
+        <v>45929</v>
+      </c>
+      <c r="D70" s="6">
+        <v>5</v>
       </c>
       <c r="E70">
         <v>1</v>
@@ -2730,38 +2631,39 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>159</v>
+        <v>119</v>
       </c>
       <c r="B71" t="s">
-        <v>166</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="D71" s="2" t="s">
-        <v>267</v>
+        <v>116</v>
+      </c>
+      <c r="C71" s="3">
+        <v>45929</v>
+      </c>
+      <c r="D71" s="6">
+        <v>5</v>
       </c>
       <c r="E71">
         <v>1</v>
       </c>
+      <c r="F71"/>
       <c r="G71">
         <v>0</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>160</v>
+        <v>120</v>
       </c>
       <c r="B72" t="s">
-        <v>165</v>
-      </c>
-      <c r="C72" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="D72" s="2" t="s">
-        <v>267</v>
+        <v>124</v>
+      </c>
+      <c r="C72" s="3">
+        <v>45930</v>
+      </c>
+      <c r="D72" s="6">
+        <v>5</v>
       </c>
       <c r="E72">
         <v>1</v>
@@ -2771,60 +2673,59 @@
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A73" t="s">
-        <v>167</v>
-      </c>
-      <c r="B73" t="s">
-        <v>168</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="D73" s="2" t="s">
-        <v>267</v>
-      </c>
-      <c r="E73">
-        <v>1</v>
-      </c>
+      <c r="A73" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C73" s="4">
+        <v>45930</v>
+      </c>
+      <c r="D73" s="7">
+        <v>5</v>
+      </c>
+      <c r="E73" s="2">
+        <v>1</v>
+      </c>
+      <c r="F73" s="2"/>
       <c r="G73">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>170</v>
+        <v>122</v>
       </c>
       <c r="B74" t="s">
-        <v>174</v>
-      </c>
-      <c r="C74" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="D74" s="2" t="s">
-        <v>267</v>
+        <v>126</v>
+      </c>
+      <c r="C74" s="3">
+        <v>45931</v>
+      </c>
+      <c r="D74" s="6">
+        <v>5</v>
       </c>
       <c r="E74">
         <v>1</v>
       </c>
-      <c r="F74" t="s">
-        <v>254</v>
-      </c>
+      <c r="F74"/>
       <c r="G74">
         <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>171</v>
+        <v>127</v>
       </c>
       <c r="B75" t="s">
-        <v>175</v>
-      </c>
-      <c r="C75" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="D75" s="2" t="s">
-        <v>267</v>
+        <v>128</v>
+      </c>
+      <c r="C75" s="3">
+        <v>45932</v>
+      </c>
+      <c r="D75" s="6">
+        <v>5</v>
       </c>
       <c r="E75">
         <v>1</v>
@@ -2835,22 +2736,22 @@
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>172</v>
+        <v>129</v>
       </c>
       <c r="B76" t="s">
-        <v>176</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="D76" s="2" t="s">
-        <v>267</v>
+        <v>132</v>
+      </c>
+      <c r="C76" s="3">
+        <v>45932</v>
+      </c>
+      <c r="D76" s="6">
+        <v>5</v>
       </c>
       <c r="E76">
         <v>1</v>
       </c>
       <c r="F76" t="s">
-        <v>254</v>
+        <v>199</v>
       </c>
       <c r="G76">
         <v>0</v>
@@ -2858,22 +2759,22 @@
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>173</v>
+        <v>130</v>
       </c>
       <c r="B77" t="s">
-        <v>177</v>
-      </c>
-      <c r="C77" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="D77" s="2" t="s">
-        <v>267</v>
+        <v>133</v>
+      </c>
+      <c r="C77" s="3">
+        <v>45932</v>
+      </c>
+      <c r="D77" s="6">
+        <v>5</v>
       </c>
       <c r="E77">
         <v>1</v>
       </c>
       <c r="F77" t="s">
-        <v>254</v>
+        <v>199</v>
       </c>
       <c r="G77">
         <v>0</v>
@@ -2881,19 +2782,22 @@
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>179</v>
+        <v>131</v>
       </c>
       <c r="B78" t="s">
-        <v>182</v>
-      </c>
-      <c r="C78" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="D78" s="2" t="s">
-        <v>267</v>
+        <v>134</v>
+      </c>
+      <c r="C78" s="3">
+        <v>45932</v>
+      </c>
+      <c r="D78" s="6">
+        <v>5</v>
       </c>
       <c r="E78">
         <v>1</v>
+      </c>
+      <c r="F78" t="s">
+        <v>199</v>
       </c>
       <c r="G78">
         <v>0</v>
@@ -2901,22 +2805,22 @@
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>180</v>
+        <v>166</v>
       </c>
       <c r="B79" t="s">
-        <v>181</v>
-      </c>
-      <c r="C79" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="D79" s="2" t="s">
-        <v>267</v>
+        <v>203</v>
+      </c>
+      <c r="C79" s="3">
+        <v>45933</v>
+      </c>
+      <c r="D79" s="6">
+        <v>5</v>
       </c>
       <c r="E79">
         <v>1</v>
       </c>
       <c r="F79" t="s">
-        <v>254</v>
+        <v>199</v>
       </c>
       <c r="G79">
         <v>0</v>
@@ -2924,16 +2828,16 @@
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>186</v>
+        <v>135</v>
       </c>
       <c r="B80" t="s">
-        <v>183</v>
-      </c>
-      <c r="C80" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="D80" s="2" t="s">
-        <v>268</v>
+        <v>138</v>
+      </c>
+      <c r="C80" s="3">
+        <v>45934</v>
+      </c>
+      <c r="D80" s="6">
+        <v>5</v>
       </c>
       <c r="E80">
         <v>1</v>
@@ -2944,36 +2848,39 @@
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>185</v>
+        <v>136</v>
       </c>
       <c r="B81" t="s">
-        <v>190</v>
-      </c>
-      <c r="C81" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="D81" s="2" t="s">
-        <v>268</v>
+        <v>137</v>
+      </c>
+      <c r="C81" s="3">
+        <v>45934</v>
+      </c>
+      <c r="D81" s="6">
+        <v>5</v>
       </c>
       <c r="E81">
         <v>1</v>
       </c>
+      <c r="F81" t="s">
+        <v>199</v>
+      </c>
       <c r="G81">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>187</v>
+        <v>141</v>
       </c>
       <c r="B82" t="s">
-        <v>191</v>
-      </c>
-      <c r="C82" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="D82" s="2" t="s">
-        <v>268</v>
+        <v>139</v>
+      </c>
+      <c r="C82" s="3">
+        <v>45936</v>
+      </c>
+      <c r="D82" s="6">
+        <v>6</v>
       </c>
       <c r="E82">
         <v>1</v>
@@ -2982,44 +2889,42 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>188</v>
+        <v>140</v>
       </c>
       <c r="B83" t="s">
-        <v>192</v>
-      </c>
-      <c r="C83" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="D83" s="2" t="s">
-        <v>268</v>
+        <v>144</v>
+      </c>
+      <c r="C83" s="3">
+        <v>45936</v>
+      </c>
+      <c r="D83" s="6">
+        <v>6</v>
       </c>
       <c r="E83">
         <v>1</v>
       </c>
+      <c r="F83"/>
       <c r="G83">
         <v>0</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>189</v>
+        <v>142</v>
       </c>
       <c r="B84" t="s">
-        <v>193</v>
-      </c>
-      <c r="C84" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="D84" s="2" t="s">
-        <v>268</v>
+        <v>145</v>
+      </c>
+      <c r="C84" s="3">
+        <v>45936</v>
+      </c>
+      <c r="D84" s="6">
+        <v>6</v>
       </c>
       <c r="E84">
         <v>1</v>
-      </c>
-      <c r="F84" t="s">
-        <v>254</v>
       </c>
       <c r="G84">
         <v>0</v>
@@ -3027,105 +2932,104 @@
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>196</v>
+        <v>143</v>
       </c>
       <c r="B85" t="s">
-        <v>195</v>
-      </c>
-      <c r="C85" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="D85" s="2" t="s">
-        <v>268</v>
+        <v>146</v>
+      </c>
+      <c r="C85" s="3">
+        <v>45936</v>
+      </c>
+      <c r="D85" s="6">
+        <v>6</v>
       </c>
       <c r="E85">
         <v>1</v>
       </c>
-      <c r="F85" t="s">
-        <v>254</v>
-      </c>
       <c r="G85">
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>197</v>
+        <v>148</v>
       </c>
       <c r="B86" t="s">
-        <v>198</v>
-      </c>
-      <c r="C86" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="D86" s="2" t="s">
-        <v>268</v>
+        <v>147</v>
+      </c>
+      <c r="C86" s="3">
+        <v>45937</v>
+      </c>
+      <c r="D86" s="6">
+        <v>6</v>
       </c>
       <c r="E86">
         <v>1</v>
       </c>
+      <c r="F86" t="s">
+        <v>199</v>
+      </c>
       <c r="G86">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>200</v>
+        <v>149</v>
       </c>
       <c r="B87" t="s">
-        <v>271</v>
-      </c>
-      <c r="C87" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="D87" s="2" t="s">
-        <v>268</v>
+        <v>150</v>
+      </c>
+      <c r="C87" s="3">
+        <v>45938</v>
+      </c>
+      <c r="D87" s="6">
+        <v>6</v>
       </c>
       <c r="E87">
         <v>1</v>
       </c>
+      <c r="F87"/>
       <c r="G87">
         <v>0</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A88" t="s">
-        <v>201</v>
-      </c>
-      <c r="B88" t="s">
-        <v>202</v>
-      </c>
-      <c r="C88" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="D88" s="2" t="s">
-        <v>268</v>
-      </c>
-      <c r="E88">
-        <v>1</v>
-      </c>
+      <c r="A88" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="C88" s="4">
+        <v>45938</v>
+      </c>
+      <c r="D88" s="7">
+        <v>6</v>
+      </c>
+      <c r="E88" s="2">
+        <v>1</v>
+      </c>
+      <c r="F88" s="2"/>
       <c r="G88">
         <v>0</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>204</v>
+        <v>151</v>
       </c>
       <c r="B89" t="s">
-        <v>210</v>
-      </c>
-      <c r="C89" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="D89" s="2" t="s">
-        <v>268</v>
+        <v>152</v>
+      </c>
+      <c r="C89" s="3">
+        <v>45938</v>
+      </c>
+      <c r="D89" s="6">
+        <v>6</v>
       </c>
       <c r="E89">
         <v>1</v>
-      </c>
-      <c r="F89" t="s">
-        <v>254</v>
       </c>
       <c r="G89">
         <v>0</v>
@@ -3133,22 +3037,22 @@
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>205</v>
+        <v>153</v>
       </c>
       <c r="B90" t="s">
-        <v>211</v>
-      </c>
-      <c r="C90" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="D90" s="2" t="s">
-        <v>268</v>
+        <v>159</v>
+      </c>
+      <c r="C90" s="3">
+        <v>45939</v>
+      </c>
+      <c r="D90" s="6">
+        <v>6</v>
       </c>
       <c r="E90">
         <v>1</v>
       </c>
       <c r="F90" t="s">
-        <v>254</v>
+        <v>199</v>
       </c>
       <c r="G90">
         <v>0</v>
@@ -3156,19 +3060,22 @@
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>206</v>
+        <v>154</v>
       </c>
       <c r="B91" t="s">
-        <v>212</v>
-      </c>
-      <c r="C91" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="D91" s="2" t="s">
-        <v>268</v>
+        <v>160</v>
+      </c>
+      <c r="C91" s="3">
+        <v>45939</v>
+      </c>
+      <c r="D91" s="6">
+        <v>6</v>
       </c>
       <c r="E91">
         <v>1</v>
+      </c>
+      <c r="F91" t="s">
+        <v>199</v>
       </c>
       <c r="G91">
         <v>0</v>
@@ -3176,22 +3083,19 @@
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>207</v>
+        <v>155</v>
       </c>
       <c r="B92" t="s">
-        <v>213</v>
-      </c>
-      <c r="C92" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="D92" s="2" t="s">
-        <v>268</v>
+        <v>161</v>
+      </c>
+      <c r="C92" s="3">
+        <v>45939</v>
+      </c>
+      <c r="D92" s="6">
+        <v>6</v>
       </c>
       <c r="E92">
         <v>1</v>
-      </c>
-      <c r="F92" t="s">
-        <v>254</v>
       </c>
       <c r="G92">
         <v>0</v>
@@ -3199,19 +3103,22 @@
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>208</v>
+        <v>156</v>
       </c>
       <c r="B93" t="s">
-        <v>214</v>
-      </c>
-      <c r="C93" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="D93" s="2" t="s">
-        <v>268</v>
+        <v>162</v>
+      </c>
+      <c r="C93" s="3">
+        <v>45939</v>
+      </c>
+      <c r="D93" s="6">
+        <v>6</v>
       </c>
       <c r="E93">
         <v>1</v>
+      </c>
+      <c r="F93" t="s">
+        <v>199</v>
       </c>
       <c r="G93">
         <v>0</v>
@@ -3219,16 +3126,16 @@
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>209</v>
+        <v>157</v>
       </c>
       <c r="B94" t="s">
-        <v>215</v>
-      </c>
-      <c r="C94" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="D94" s="2" t="s">
-        <v>268</v>
+        <v>163</v>
+      </c>
+      <c r="C94" s="3">
+        <v>45939</v>
+      </c>
+      <c r="D94" s="6">
+        <v>6</v>
       </c>
       <c r="E94">
         <v>1</v>
@@ -3239,16 +3146,16 @@
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>217</v>
+        <v>158</v>
       </c>
       <c r="B95" t="s">
-        <v>219</v>
-      </c>
-      <c r="C95" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="D95" s="2" t="s">
-        <v>268</v>
+        <v>164</v>
+      </c>
+      <c r="C95" s="3">
+        <v>45939</v>
+      </c>
+      <c r="D95" s="6">
+        <v>6</v>
       </c>
       <c r="E95">
         <v>1</v>
@@ -3259,59 +3166,57 @@
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>218</v>
+        <v>165</v>
       </c>
       <c r="B96" t="s">
-        <v>260</v>
-      </c>
-      <c r="C96" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="D96" s="2" t="s">
-        <v>268</v>
+        <v>167</v>
+      </c>
+      <c r="C96" s="3">
+        <v>45941</v>
+      </c>
+      <c r="D96" s="6">
+        <v>6</v>
       </c>
       <c r="E96">
         <v>1</v>
       </c>
-      <c r="F96" t="s">
-        <v>254</v>
-      </c>
       <c r="G96">
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>220</v>
+        <v>170</v>
       </c>
       <c r="B97" t="s">
-        <v>221</v>
-      </c>
-      <c r="C97" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="D97" s="2" t="s">
-        <v>269</v>
+        <v>180</v>
+      </c>
+      <c r="C97" s="3">
+        <v>45945</v>
+      </c>
+      <c r="D97" s="6">
+        <v>7</v>
       </c>
       <c r="E97">
         <v>1</v>
       </c>
+      <c r="F97"/>
       <c r="G97">
         <v>0</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>223</v>
+        <v>175</v>
       </c>
       <c r="B98" t="s">
-        <v>233</v>
-      </c>
-      <c r="C98" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="D98" s="2" t="s">
-        <v>269</v>
+        <v>185</v>
+      </c>
+      <c r="C98" s="3">
+        <v>45945</v>
+      </c>
+      <c r="D98" s="6">
+        <v>7</v>
       </c>
       <c r="E98">
         <v>1</v>
@@ -3322,16 +3227,16 @@
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>224</v>
+        <v>171</v>
       </c>
       <c r="B99" t="s">
-        <v>234</v>
-      </c>
-      <c r="C99" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="D99" s="2" t="s">
-        <v>269</v>
+        <v>181</v>
+      </c>
+      <c r="C99" s="3">
+        <v>45945</v>
+      </c>
+      <c r="D99" s="6">
+        <v>7</v>
       </c>
       <c r="E99">
         <v>1</v>
@@ -3342,22 +3247,22 @@
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>225</v>
+        <v>176</v>
       </c>
       <c r="B100" t="s">
-        <v>235</v>
-      </c>
-      <c r="C100" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="D100" s="2" t="s">
-        <v>269</v>
+        <v>186</v>
+      </c>
+      <c r="C100" s="3">
+        <v>45945</v>
+      </c>
+      <c r="D100" s="6">
+        <v>7</v>
       </c>
       <c r="E100">
         <v>1</v>
       </c>
       <c r="F100" t="s">
-        <v>254</v>
+        <v>199</v>
       </c>
       <c r="G100">
         <v>0</v>
@@ -3365,16 +3270,16 @@
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>226</v>
+        <v>177</v>
       </c>
       <c r="B101" t="s">
-        <v>236</v>
-      </c>
-      <c r="C101" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="D101" s="2" t="s">
-        <v>269</v>
+        <v>187</v>
+      </c>
+      <c r="C101" s="3">
+        <v>45945</v>
+      </c>
+      <c r="D101" s="6">
+        <v>7</v>
       </c>
       <c r="E101">
         <v>1</v>
@@ -3385,16 +3290,16 @@
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>227</v>
+        <v>178</v>
       </c>
       <c r="B102" t="s">
-        <v>237</v>
-      </c>
-      <c r="C102" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="D102" s="2" t="s">
-        <v>269</v>
+        <v>188</v>
+      </c>
+      <c r="C102" s="3">
+        <v>45945</v>
+      </c>
+      <c r="D102" s="6">
+        <v>7</v>
       </c>
       <c r="E102">
         <v>1</v>
@@ -3405,61 +3310,62 @@
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
+        <v>179</v>
+      </c>
+      <c r="B103" t="s">
+        <v>189</v>
+      </c>
+      <c r="C103" s="3">
+        <v>45945</v>
+      </c>
+      <c r="D103" s="6">
+        <v>7</v>
+      </c>
+      <c r="E103">
+        <v>1</v>
+      </c>
+      <c r="F103" t="s">
+        <v>199</v>
+      </c>
+      <c r="G103">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A104" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="C104" s="5">
+        <v>45946</v>
+      </c>
+      <c r="D104" s="8">
+        <v>7</v>
+      </c>
+      <c r="E104" s="1">
+        <v>1</v>
+      </c>
+      <c r="F104" s="1"/>
+      <c r="G104">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A105" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="B103" t="s">
-        <v>238</v>
-      </c>
-      <c r="C103" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="D103" s="2" t="s">
-        <v>269</v>
-      </c>
-      <c r="E103">
-        <v>1</v>
-      </c>
-      <c r="G103">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A104" t="s">
+      <c r="B105" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="B104" t="s">
-        <v>239</v>
-      </c>
-      <c r="C104" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="D104" s="2" t="s">
-        <v>269</v>
-      </c>
-      <c r="E104">
-        <v>1</v>
-      </c>
-      <c r="F104" t="s">
-        <v>254</v>
-      </c>
-      <c r="G104">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A105" t="s">
-        <v>230</v>
-      </c>
-      <c r="B105" t="s">
-        <v>240</v>
-      </c>
-      <c r="C105" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="D105" s="2" t="s">
-        <v>269</v>
-      </c>
-      <c r="E105">
+      <c r="C105" s="4">
+        <v>45946</v>
+      </c>
+      <c r="D105" s="7">
+        <v>7</v>
+      </c>
+      <c r="E105" s="2">
         <v>1</v>
       </c>
       <c r="G105">
@@ -3467,109 +3373,109 @@
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A106" t="s">
-        <v>231</v>
-      </c>
-      <c r="B106" t="s">
-        <v>241</v>
-      </c>
-      <c r="C106" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="D106" s="2" t="s">
-        <v>269</v>
-      </c>
-      <c r="E106">
-        <v>1</v>
-      </c>
+      <c r="A106" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="C106" s="4">
+        <v>45946</v>
+      </c>
+      <c r="D106" s="7">
+        <v>7</v>
+      </c>
+      <c r="E106" s="2">
+        <v>1</v>
+      </c>
+      <c r="F106" s="2"/>
       <c r="G106">
         <v>0</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>232</v>
+        <v>172</v>
       </c>
       <c r="B107" t="s">
-        <v>242</v>
-      </c>
-      <c r="C107" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="D107" s="2" t="s">
-        <v>269</v>
+        <v>182</v>
+      </c>
+      <c r="C107" s="3">
+        <v>45946</v>
+      </c>
+      <c r="D107" s="6">
+        <v>7</v>
       </c>
       <c r="E107">
         <v>1</v>
       </c>
       <c r="F107" t="s">
-        <v>254</v>
+        <v>199</v>
       </c>
       <c r="G107">
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>243</v>
+        <v>173</v>
       </c>
       <c r="B108" t="s">
-        <v>245</v>
-      </c>
-      <c r="C108" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="D108" s="2" t="s">
-        <v>269</v>
+        <v>183</v>
+      </c>
+      <c r="C108" s="3">
+        <v>45946</v>
+      </c>
+      <c r="D108" s="6">
+        <v>7</v>
       </c>
       <c r="E108">
         <v>1</v>
       </c>
+      <c r="F108"/>
       <c r="G108">
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>246</v>
+        <v>174</v>
       </c>
       <c r="B109" t="s">
-        <v>249</v>
-      </c>
-      <c r="C109" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="D109" s="2" t="s">
-        <v>270</v>
+        <v>184</v>
+      </c>
+      <c r="C109" s="3">
+        <v>45946</v>
+      </c>
+      <c r="D109" s="6">
+        <v>7</v>
       </c>
       <c r="E109">
         <v>1</v>
       </c>
-      <c r="F109" t="s">
-        <v>254</v>
-      </c>
+      <c r="F109"/>
       <c r="G109">
         <v>0</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>247</v>
+        <v>193</v>
       </c>
       <c r="B110" t="s">
-        <v>250</v>
-      </c>
-      <c r="C110" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="D110" s="2" t="s">
-        <v>270</v>
+        <v>196</v>
+      </c>
+      <c r="C110" s="3">
+        <v>45955</v>
+      </c>
+      <c r="D110" s="6">
+        <v>8</v>
       </c>
       <c r="E110">
         <v>1</v>
       </c>
       <c r="F110" t="s">
-        <v>254</v>
+        <v>199</v>
       </c>
       <c r="G110">
         <v>0</v>
@@ -3577,32 +3483,55 @@
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>248</v>
+        <v>192</v>
       </c>
       <c r="B111" t="s">
-        <v>251</v>
-      </c>
-      <c r="C111" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="D111" s="2" t="s">
-        <v>270</v>
+        <v>195</v>
+      </c>
+      <c r="C111" s="3">
+        <v>45955</v>
+      </c>
+      <c r="D111" s="6">
+        <v>8</v>
       </c>
       <c r="E111">
         <v>1</v>
       </c>
       <c r="F111" t="s">
-        <v>254</v>
+        <v>199</v>
       </c>
       <c r="G111">
         <v>0</v>
       </c>
     </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A112" t="s">
+        <v>194</v>
+      </c>
+      <c r="B112" t="s">
+        <v>197</v>
+      </c>
+      <c r="C112" s="3">
+        <v>228576</v>
+      </c>
+      <c r="D112" s="6">
+        <v>8</v>
+      </c>
+      <c r="E112">
+        <v>1</v>
+      </c>
+      <c r="F112" t="s">
+        <v>199</v>
+      </c>
+      <c r="G112">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G121">
+    <sortCondition ref="C2:C121"/>
+  </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <ignoredErrors>
-    <ignoredError sqref="D2 D3:D6 D8:D26" numberStoredAsText="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Start getting 2025 results
</commit_message>
<xml_diff>
--- a/2025/meet_list_data_ready.xlsx
+++ b/2025/meet_list_data_ready.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dburk\Documents\GitHub\sdxc-data\2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECA4E173-3CBD-4178-8FF6-DD2830A03305}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A541F465-8530-417B-8D0B-1A1AED414644}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{1EB159B1-87E3-4E73-9839-0175057112CF}"/>
+    <workbookView xWindow="2268" yWindow="1560" windowWidth="17280" windowHeight="10680" xr2:uid="{1EB159B1-87E3-4E73-9839-0175057112CF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="228">
   <si>
     <t>official_meet_name</t>
   </si>
@@ -630,12 +630,6 @@
   </si>
   <si>
     <t>sdhsaa_aa</t>
-  </si>
-  <si>
-    <t>source</t>
-  </si>
-  <si>
-    <t>DT</t>
   </si>
   <si>
     <t>White River Presige Run</t>
@@ -775,17 +769,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1125,2410 +1114,2239 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BABB3D95-ED19-41E8-9BC3-61C8F80036A4}">
-  <dimension ref="A1:G112"/>
+  <dimension ref="A1:F112"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J12" sqref="J12"/>
+      <selection pane="bottomLeft" activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="29.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
-        <v>205</v>
+      <c r="D1" s="4" t="s">
+        <v>203</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>198</v>
-      </c>
-      <c r="G1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="2">
         <v>45897</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2" s="4">
         <v>1</v>
       </c>
       <c r="E2">
         <v>1</v>
       </c>
-      <c r="F2" t="s">
-        <v>199</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="2">
         <v>45897</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="4">
         <v>1</v>
       </c>
       <c r="E3">
         <v>1</v>
       </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>204</v>
-      </c>
-      <c r="C4" s="3">
+        <v>202</v>
+      </c>
+      <c r="C4" s="2">
         <v>45897</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="4">
         <v>1</v>
       </c>
       <c r="E4">
         <v>0</v>
       </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>19</v>
       </c>
       <c r="B5" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="2">
         <v>45897</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="4">
         <v>1</v>
       </c>
       <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B6" t="s">
-        <v>207</v>
-      </c>
-      <c r="C6" s="3">
+        <v>205</v>
+      </c>
+      <c r="C6" s="2">
         <v>45897</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="4">
         <v>1</v>
       </c>
       <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="F6"/>
-      <c r="G6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>9</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="2">
         <v>45897</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="4">
         <v>1</v>
       </c>
       <c r="E7">
         <v>0</v>
       </c>
-      <c r="F7" t="s">
-        <v>199</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B8" t="s">
-        <v>209</v>
-      </c>
-      <c r="C8" s="3">
+        <v>207</v>
+      </c>
+      <c r="C8" s="2">
         <v>45898</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="4">
         <v>1</v>
       </c>
       <c r="E8">
         <v>1</v>
       </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>202</v>
-      </c>
-      <c r="C9" s="3">
+        <v>200</v>
+      </c>
+      <c r="C9" s="2">
         <v>45898</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="4">
         <v>1</v>
       </c>
       <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9" t="s">
-        <v>199</v>
-      </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>11</v>
       </c>
       <c r="B10" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="2">
         <v>45898</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="4">
         <v>1</v>
       </c>
       <c r="E10">
         <v>0</v>
       </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>13</v>
       </c>
       <c r="B11" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="2">
         <v>45898</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="4">
         <v>1</v>
       </c>
       <c r="E11">
         <v>1</v>
       </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>21</v>
       </c>
       <c r="B12" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="2">
         <v>45902</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="4">
         <v>1</v>
       </c>
       <c r="E12">
         <v>1</v>
       </c>
-      <c r="F12" t="s">
-        <v>199</v>
-      </c>
-      <c r="G12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>23</v>
       </c>
       <c r="B13" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="2">
         <v>45902</v>
       </c>
-      <c r="D13" s="6">
+      <c r="D13" s="4">
         <v>1</v>
       </c>
       <c r="E13">
         <v>1</v>
       </c>
-      <c r="G13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>25</v>
       </c>
       <c r="B14" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="2">
         <v>45902</v>
       </c>
-      <c r="D14" s="6">
+      <c r="D14" s="4">
         <v>1</v>
       </c>
       <c r="E14">
         <v>1</v>
       </c>
-      <c r="F14" t="s">
-        <v>199</v>
-      </c>
-      <c r="G14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>27</v>
       </c>
       <c r="B15" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15" s="2">
         <v>45902</v>
       </c>
-      <c r="D15" s="6">
-        <v>1</v>
-      </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
-      <c r="F15" t="s">
-        <v>199</v>
-      </c>
-      <c r="G15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D15" s="4">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B16" t="s">
-        <v>211</v>
-      </c>
-      <c r="C16" s="3">
+        <v>209</v>
+      </c>
+      <c r="C16" s="2">
         <v>45902</v>
       </c>
-      <c r="D16" s="6">
-        <v>1</v>
-      </c>
-      <c r="E16">
-        <v>1</v>
-      </c>
-      <c r="G16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D16" s="4">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>29</v>
       </c>
       <c r="B17" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C17" s="2">
         <v>45904</v>
       </c>
-      <c r="D17" s="6">
-        <v>1</v>
-      </c>
-      <c r="E17">
-        <v>1</v>
-      </c>
-      <c r="G17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D17" s="4">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>33</v>
       </c>
       <c r="B18" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C18" s="2">
         <v>45905</v>
       </c>
-      <c r="D18" s="6">
-        <v>1</v>
-      </c>
-      <c r="E18">
-        <v>1</v>
-      </c>
-      <c r="F18" t="s">
-        <v>199</v>
-      </c>
-      <c r="G18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D18" s="4">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B19" t="s">
         <v>37</v>
       </c>
-      <c r="C19" s="3">
+      <c r="C19" s="2">
         <v>45905</v>
       </c>
-      <c r="D19" s="6">
-        <v>1</v>
-      </c>
-      <c r="E19">
-        <v>1</v>
-      </c>
-      <c r="F19" t="s">
-        <v>199</v>
-      </c>
-      <c r="G19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D19" s="4">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>31</v>
       </c>
       <c r="B20" t="s">
         <v>32</v>
       </c>
-      <c r="C20" s="3">
+      <c r="C20" s="2">
         <v>45905</v>
       </c>
-      <c r="D20" s="6">
-        <v>1</v>
-      </c>
-      <c r="E20">
-        <v>1</v>
-      </c>
-      <c r="F20"/>
-      <c r="G20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D20" s="4">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>35</v>
       </c>
       <c r="B21" t="s">
         <v>36</v>
       </c>
-      <c r="C21" s="3">
+      <c r="C21" s="2">
         <v>45905</v>
       </c>
-      <c r="D21" s="6">
-        <v>1</v>
-      </c>
-      <c r="E21">
-        <v>1</v>
-      </c>
-      <c r="F21" t="s">
-        <v>199</v>
-      </c>
-      <c r="G21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
+      <c r="D21" s="4">
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>15</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" t="s">
         <v>16</v>
       </c>
-      <c r="C22" s="4">
+      <c r="C22" s="2">
         <v>45906</v>
       </c>
-      <c r="D22" s="7">
-        <v>1</v>
-      </c>
-      <c r="E22" s="2">
-        <v>1</v>
-      </c>
-      <c r="F22" s="2"/>
-      <c r="G22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D22" s="4">
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>42</v>
       </c>
       <c r="B23" t="s">
         <v>43</v>
       </c>
-      <c r="C23" s="3">
+      <c r="C23" s="2">
         <v>45908</v>
       </c>
-      <c r="D23" s="6">
+      <c r="D23" s="4">
         <v>2</v>
       </c>
       <c r="E23">
         <v>1</v>
       </c>
-      <c r="F23"/>
-      <c r="G23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>40</v>
       </c>
       <c r="B24" t="s">
         <v>41</v>
       </c>
-      <c r="C24" s="3">
+      <c r="C24" s="2">
         <v>45909</v>
       </c>
-      <c r="D24" s="6">
+      <c r="D24" s="4">
         <v>2</v>
       </c>
       <c r="E24">
         <v>1</v>
       </c>
-      <c r="F24" t="s">
-        <v>199</v>
-      </c>
-      <c r="G24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B25" t="s">
-        <v>217</v>
-      </c>
-      <c r="C25" s="3">
+        <v>215</v>
+      </c>
+      <c r="C25" s="2">
         <v>45909</v>
       </c>
-      <c r="D25" s="6">
+      <c r="D25" s="4">
         <v>2</v>
       </c>
       <c r="E25">
         <v>1</v>
       </c>
-      <c r="G25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>38</v>
       </c>
       <c r="B26" t="s">
         <v>39</v>
       </c>
-      <c r="C26" s="3">
+      <c r="C26" s="2">
         <v>45909</v>
       </c>
-      <c r="D26" s="6">
+      <c r="D26" s="4">
         <v>2</v>
       </c>
       <c r="E26">
         <v>1</v>
       </c>
-      <c r="F26" t="s">
-        <v>199</v>
-      </c>
-      <c r="G26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>46</v>
       </c>
       <c r="B27" t="s">
         <v>47</v>
       </c>
-      <c r="C27" s="3">
+      <c r="C27" s="2">
         <v>45910</v>
       </c>
-      <c r="D27" s="6">
+      <c r="D27" s="4">
         <v>2</v>
       </c>
       <c r="E27">
         <v>1</v>
       </c>
-      <c r="G27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B28" t="s">
-        <v>215</v>
-      </c>
-      <c r="C28" s="3">
+        <v>213</v>
+      </c>
+      <c r="C28" s="2">
         <v>45910</v>
       </c>
-      <c r="D28" s="6">
+      <c r="D28" s="4">
         <v>2</v>
       </c>
       <c r="E28">
         <v>1</v>
       </c>
-      <c r="G28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>48</v>
       </c>
       <c r="B29" t="s">
         <v>49</v>
       </c>
-      <c r="C29" s="3">
+      <c r="C29" s="2">
         <v>45911</v>
       </c>
-      <c r="D29" s="6">
+      <c r="D29" s="4">
         <v>2</v>
       </c>
       <c r="E29">
         <v>1</v>
       </c>
-      <c r="F29" t="s">
-        <v>199</v>
-      </c>
-      <c r="G29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>50</v>
       </c>
       <c r="B30" t="s">
         <v>51</v>
       </c>
-      <c r="C30" s="3">
+      <c r="C30" s="2">
         <v>45911</v>
       </c>
-      <c r="D30" s="6">
+      <c r="D30" s="4">
         <v>2</v>
       </c>
       <c r="E30">
         <v>1</v>
       </c>
-      <c r="G30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>52</v>
       </c>
       <c r="B31" t="s">
         <v>53</v>
       </c>
-      <c r="C31" s="3">
+      <c r="C31" s="2">
         <v>45911</v>
       </c>
-      <c r="D31" s="6">
+      <c r="D31" s="4">
         <v>2</v>
       </c>
       <c r="E31">
         <v>1</v>
       </c>
-      <c r="G31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>54</v>
       </c>
       <c r="B32" t="s">
         <v>55</v>
       </c>
-      <c r="C32" s="3">
+      <c r="C32" s="2">
         <v>45912</v>
       </c>
-      <c r="D32" s="6">
+      <c r="D32" s="4">
         <v>2</v>
       </c>
       <c r="E32">
         <v>1</v>
       </c>
-      <c r="F32" t="s">
-        <v>199</v>
-      </c>
-      <c r="G32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>56</v>
       </c>
       <c r="B33" t="s">
         <v>57</v>
       </c>
-      <c r="C33" s="3">
+      <c r="C33" s="2">
         <v>45913</v>
       </c>
-      <c r="D33" s="6">
+      <c r="D33" s="4">
         <v>2</v>
       </c>
       <c r="E33">
         <v>1</v>
       </c>
-      <c r="G33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>58</v>
       </c>
       <c r="B34" t="s">
         <v>59</v>
       </c>
-      <c r="C34" s="3">
+      <c r="C34" s="2">
         <v>45913</v>
       </c>
-      <c r="D34" s="6">
+      <c r="D34" s="4">
         <v>2</v>
       </c>
       <c r="E34">
         <v>1</v>
       </c>
-      <c r="G34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>60</v>
       </c>
       <c r="B35" t="s">
         <v>61</v>
       </c>
-      <c r="C35" s="3">
+      <c r="C35" s="2">
         <v>45913</v>
       </c>
-      <c r="D35" s="6">
+      <c r="D35" s="4">
         <v>2</v>
       </c>
       <c r="E35">
         <v>1</v>
       </c>
-      <c r="F35" t="s">
-        <v>199</v>
-      </c>
-      <c r="G35">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B36" t="s">
         <v>62</v>
       </c>
-      <c r="C36" s="3">
+      <c r="C36" s="2">
         <v>45913</v>
       </c>
-      <c r="D36" s="6">
+      <c r="D36" s="4">
         <v>2</v>
       </c>
       <c r="E36">
         <v>1</v>
       </c>
-      <c r="G36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="F36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>63</v>
       </c>
       <c r="B37" t="s">
         <v>64</v>
       </c>
-      <c r="C37" s="3">
+      <c r="C37" s="2">
         <v>45915</v>
       </c>
-      <c r="D37" s="6">
+      <c r="D37" s="4">
         <v>3</v>
       </c>
       <c r="E37">
         <v>1</v>
       </c>
-      <c r="F37"/>
-      <c r="G37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>65</v>
       </c>
       <c r="B38" t="s">
         <v>66</v>
       </c>
-      <c r="C38" s="3">
+      <c r="C38" s="2">
         <v>45915</v>
       </c>
-      <c r="D38" s="6">
+      <c r="D38" s="4">
         <v>3</v>
       </c>
       <c r="E38">
         <v>1</v>
       </c>
-      <c r="G38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>67</v>
       </c>
       <c r="B39" t="s">
         <v>68</v>
       </c>
-      <c r="C39" s="3">
+      <c r="C39" s="2">
         <v>45915</v>
       </c>
-      <c r="D39" s="6">
+      <c r="D39" s="4">
         <v>3</v>
       </c>
       <c r="E39">
         <v>1</v>
       </c>
-      <c r="G39">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>69</v>
       </c>
       <c r="B40" t="s">
         <v>70</v>
       </c>
-      <c r="C40" s="3">
+      <c r="C40" s="2">
         <v>45915</v>
       </c>
-      <c r="D40" s="6">
+      <c r="D40" s="4">
         <v>3</v>
       </c>
       <c r="E40">
         <v>1</v>
       </c>
-      <c r="G40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B41" t="s">
-        <v>201</v>
-      </c>
-      <c r="C41" s="3">
+        <v>199</v>
+      </c>
+      <c r="C41" s="2">
         <v>45915</v>
       </c>
-      <c r="D41" s="6">
+      <c r="D41" s="4">
         <v>3</v>
       </c>
       <c r="E41">
         <v>1</v>
       </c>
-      <c r="F41" t="s">
-        <v>199</v>
-      </c>
-      <c r="G41">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>71</v>
       </c>
       <c r="B42" t="s">
         <v>72</v>
       </c>
-      <c r="C42" s="3">
+      <c r="C42" s="2">
         <v>45917</v>
       </c>
-      <c r="D42" s="6">
+      <c r="D42" s="4">
         <v>3</v>
       </c>
       <c r="E42">
         <v>1</v>
       </c>
-      <c r="G42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>99</v>
       </c>
       <c r="B43" t="s">
         <v>101</v>
       </c>
-      <c r="C43" s="3">
+      <c r="C43" s="2">
         <v>45917</v>
       </c>
-      <c r="D43" s="6">
+      <c r="D43" s="4">
         <v>3</v>
       </c>
       <c r="E43">
         <v>1</v>
       </c>
-      <c r="G43">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>73</v>
       </c>
       <c r="B44" t="s">
         <v>74</v>
       </c>
-      <c r="C44" s="3">
+      <c r="C44" s="2">
         <v>45918</v>
       </c>
-      <c r="D44" s="6">
+      <c r="D44" s="4">
         <v>3</v>
       </c>
       <c r="E44">
         <v>1</v>
       </c>
-      <c r="G44">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="F44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>75</v>
       </c>
       <c r="B45" t="s">
         <v>76</v>
       </c>
-      <c r="C45" s="3">
+      <c r="C45" s="2">
         <v>45918</v>
       </c>
-      <c r="D45" s="6">
+      <c r="D45" s="4">
         <v>3</v>
       </c>
       <c r="E45">
         <v>1</v>
       </c>
-      <c r="F45" t="s">
-        <v>199</v>
-      </c>
-      <c r="G45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>77</v>
       </c>
       <c r="B46" t="s">
         <v>78</v>
       </c>
-      <c r="C46" s="3">
+      <c r="C46" s="2">
         <v>45918</v>
       </c>
-      <c r="D46" s="6">
+      <c r="D46" s="4">
         <v>3</v>
       </c>
       <c r="E46">
         <v>1</v>
       </c>
-      <c r="G46">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B47" t="s">
         <v>79</v>
       </c>
-      <c r="C47" s="3">
+      <c r="C47" s="2">
         <v>45919</v>
       </c>
-      <c r="D47" s="6">
+      <c r="D47" s="4">
         <v>3</v>
       </c>
       <c r="E47">
         <v>1</v>
       </c>
-      <c r="F47" t="s">
-        <v>199</v>
-      </c>
-      <c r="G47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>80</v>
       </c>
       <c r="B48" t="s">
         <v>81</v>
       </c>
-      <c r="C48" s="3">
+      <c r="C48" s="2">
         <v>45920</v>
       </c>
-      <c r="D48" s="6">
+      <c r="D48" s="4">
         <v>3</v>
       </c>
       <c r="E48">
         <v>1</v>
       </c>
-      <c r="G48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>82</v>
       </c>
       <c r="B49" t="s">
         <v>83</v>
       </c>
-      <c r="C49" s="3">
+      <c r="C49" s="2">
         <v>45920</v>
       </c>
-      <c r="D49" s="6">
+      <c r="D49" s="4">
         <v>3</v>
       </c>
       <c r="E49">
         <v>1</v>
       </c>
-      <c r="F49" t="s">
-        <v>199</v>
-      </c>
-      <c r="G49">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>84</v>
       </c>
       <c r="B50" t="s">
         <v>85</v>
       </c>
-      <c r="C50" s="3">
+      <c r="C50" s="2">
         <v>45920</v>
       </c>
-      <c r="D50" s="6">
+      <c r="D50" s="4">
         <v>3</v>
       </c>
       <c r="E50">
         <v>1</v>
       </c>
-      <c r="F50" t="s">
-        <v>199</v>
-      </c>
-      <c r="G50">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>86</v>
       </c>
       <c r="B51" t="s">
         <v>87</v>
       </c>
-      <c r="C51" s="3">
+      <c r="C51" s="2">
         <v>45922</v>
       </c>
-      <c r="D51" s="6">
+      <c r="D51" s="4">
         <v>4</v>
       </c>
       <c r="E51">
         <v>1</v>
       </c>
-      <c r="F51" t="s">
-        <v>199</v>
-      </c>
-      <c r="G51">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>88</v>
       </c>
       <c r="B52" t="s">
         <v>89</v>
       </c>
-      <c r="C52" s="3">
+      <c r="C52" s="2">
         <v>45922</v>
       </c>
-      <c r="D52" s="6">
+      <c r="D52" s="4">
         <v>4</v>
       </c>
       <c r="E52">
         <v>1</v>
       </c>
-      <c r="G52">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>90</v>
       </c>
       <c r="B53" t="s">
         <v>91</v>
       </c>
-      <c r="C53" s="3">
+      <c r="C53" s="2">
         <v>45922</v>
       </c>
-      <c r="D53" s="6">
+      <c r="D53" s="4">
         <v>4</v>
       </c>
       <c r="E53">
         <v>1</v>
       </c>
-      <c r="F53" t="s">
-        <v>199</v>
-      </c>
-      <c r="G53">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>92</v>
       </c>
       <c r="B54" t="s">
         <v>93</v>
       </c>
-      <c r="C54" s="3">
+      <c r="C54" s="2">
         <v>45922</v>
       </c>
-      <c r="D54" s="6">
+      <c r="D54" s="4">
         <v>4</v>
       </c>
       <c r="E54">
         <v>1</v>
       </c>
-      <c r="G54">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B55" t="s">
-        <v>220</v>
-      </c>
-      <c r="C55" s="3">
+        <v>218</v>
+      </c>
+      <c r="C55" s="2">
         <v>45922</v>
       </c>
-      <c r="D55" s="6">
+      <c r="D55" s="4">
         <v>4</v>
       </c>
       <c r="E55">
         <v>1</v>
       </c>
-      <c r="G55">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>94</v>
       </c>
       <c r="B56" t="s">
         <v>95</v>
       </c>
-      <c r="C56" s="3">
+      <c r="C56" s="2">
         <v>45923</v>
       </c>
-      <c r="D56" s="6">
+      <c r="D56" s="4">
         <v>4</v>
       </c>
       <c r="E56">
         <v>1</v>
       </c>
-      <c r="F56" t="s">
-        <v>199</v>
-      </c>
-      <c r="G56">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A57" s="2" t="s">
+      <c r="F56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
         <v>45</v>
       </c>
-      <c r="B57" s="2" t="s">
+      <c r="B57" t="s">
         <v>44</v>
       </c>
-      <c r="C57" s="4">
+      <c r="C57" s="2">
         <v>45924</v>
       </c>
-      <c r="D57" s="7">
+      <c r="D57" s="4">
         <v>4</v>
       </c>
-      <c r="E57" s="2">
-        <v>1</v>
-      </c>
-      <c r="F57" s="2"/>
-      <c r="G57">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E57">
+        <v>1</v>
+      </c>
+      <c r="F57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>96</v>
       </c>
       <c r="B58" t="s">
         <v>97</v>
       </c>
-      <c r="C58" s="3">
+      <c r="C58" s="2">
         <v>45924</v>
       </c>
-      <c r="D58" s="6">
+      <c r="D58" s="4">
         <v>4</v>
       </c>
       <c r="E58">
         <v>1</v>
       </c>
-      <c r="G58">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>123</v>
       </c>
       <c r="B59" t="s">
-        <v>221</v>
-      </c>
-      <c r="C59" s="3">
+        <v>219</v>
+      </c>
+      <c r="C59" s="2">
         <v>45924</v>
       </c>
-      <c r="D59" s="6">
+      <c r="D59" s="4">
         <v>4</v>
       </c>
       <c r="E59">
         <v>1</v>
       </c>
-      <c r="F59" t="s">
-        <v>199</v>
-      </c>
-      <c r="G59">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>98</v>
       </c>
       <c r="B60" t="s">
         <v>100</v>
       </c>
-      <c r="C60" s="3">
+      <c r="C60" s="2">
         <v>45924</v>
       </c>
-      <c r="D60" s="6">
+      <c r="D60" s="4">
         <v>4</v>
       </c>
       <c r="E60">
         <v>1</v>
       </c>
-      <c r="G60">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>102</v>
       </c>
       <c r="B61" t="s">
         <v>106</v>
       </c>
-      <c r="C61" s="3">
+      <c r="C61" s="2">
         <v>45925</v>
       </c>
-      <c r="D61" s="6">
+      <c r="D61" s="4">
         <v>4</v>
       </c>
       <c r="E61">
         <v>1</v>
       </c>
-      <c r="F61" t="s">
-        <v>199</v>
-      </c>
-      <c r="G61">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>103</v>
       </c>
       <c r="B62" t="s">
         <v>107</v>
       </c>
-      <c r="C62" s="3">
+      <c r="C62" s="2">
         <v>45925</v>
       </c>
-      <c r="D62" s="6">
+      <c r="D62" s="4">
         <v>4</v>
       </c>
       <c r="E62">
         <v>1</v>
       </c>
-      <c r="G62">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>104</v>
       </c>
       <c r="B63" t="s">
         <v>109</v>
       </c>
-      <c r="C63" s="3">
+      <c r="C63" s="2">
         <v>45925</v>
       </c>
-      <c r="D63" s="6">
+      <c r="D63" s="4">
         <v>4</v>
       </c>
       <c r="E63">
         <v>1</v>
       </c>
-      <c r="F63" t="s">
-        <v>199</v>
-      </c>
-      <c r="G63">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>105</v>
       </c>
       <c r="B64" t="s">
         <v>108</v>
       </c>
-      <c r="C64" s="3">
+      <c r="C64" s="2">
         <v>45925</v>
       </c>
-      <c r="D64" s="6">
+      <c r="D64" s="4">
         <v>4</v>
       </c>
       <c r="E64">
         <v>1</v>
       </c>
-      <c r="G64">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>110</v>
       </c>
       <c r="B65" t="s">
         <v>111</v>
       </c>
-      <c r="C65" s="3">
+      <c r="C65" s="2">
         <v>45926</v>
       </c>
-      <c r="D65" s="6">
+      <c r="D65" s="4">
         <v>4</v>
       </c>
       <c r="E65">
         <v>1</v>
       </c>
-      <c r="F65" t="s">
-        <v>199</v>
-      </c>
-      <c r="G65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B66" t="s">
-        <v>223</v>
-      </c>
-      <c r="C66" s="3">
+        <v>221</v>
+      </c>
+      <c r="C66" s="2">
         <v>45927</v>
       </c>
-      <c r="D66" s="6">
+      <c r="D66" s="4">
         <v>4</v>
       </c>
       <c r="E66">
         <v>1</v>
       </c>
-      <c r="G66">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>112</v>
       </c>
       <c r="B67" t="s">
         <v>113</v>
       </c>
-      <c r="C67" s="3">
+      <c r="C67" s="2">
         <v>45927</v>
       </c>
-      <c r="D67" s="6">
+      <c r="D67" s="4">
         <v>4</v>
       </c>
       <c r="E67">
         <v>1</v>
       </c>
-      <c r="G67">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>118</v>
       </c>
       <c r="B68" t="s">
         <v>115</v>
       </c>
-      <c r="C68" s="3">
+      <c r="C68" s="2">
         <v>45929</v>
       </c>
-      <c r="D68" s="6">
+      <c r="D68" s="4">
         <v>5</v>
       </c>
       <c r="E68">
         <v>1</v>
       </c>
-      <c r="F68" t="s">
-        <v>199</v>
-      </c>
-      <c r="G68">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="F68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B69" t="s">
-        <v>224</v>
-      </c>
-      <c r="C69" s="3">
+        <v>222</v>
+      </c>
+      <c r="C69" s="2">
         <v>45929</v>
       </c>
-      <c r="D69" s="6">
+      <c r="D69" s="4">
         <v>5</v>
       </c>
       <c r="E69">
         <v>1</v>
       </c>
-      <c r="F69"/>
-      <c r="G69">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>117</v>
       </c>
       <c r="B70" t="s">
         <v>114</v>
       </c>
-      <c r="C70" s="3">
+      <c r="C70" s="2">
         <v>45929</v>
       </c>
-      <c r="D70" s="6">
+      <c r="D70" s="4">
         <v>5</v>
       </c>
       <c r="E70">
         <v>1</v>
       </c>
-      <c r="G70">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="F70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>119</v>
       </c>
       <c r="B71" t="s">
         <v>116</v>
       </c>
-      <c r="C71" s="3">
+      <c r="C71" s="2">
         <v>45929</v>
       </c>
-      <c r="D71" s="6">
+      <c r="D71" s="4">
         <v>5</v>
       </c>
       <c r="E71">
         <v>1</v>
       </c>
-      <c r="F71"/>
-      <c r="G71">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>120</v>
       </c>
       <c r="B72" t="s">
         <v>124</v>
       </c>
-      <c r="C72" s="3">
+      <c r="C72" s="2">
         <v>45930</v>
       </c>
-      <c r="D72" s="6">
+      <c r="D72" s="4">
         <v>5</v>
       </c>
       <c r="E72">
         <v>1</v>
       </c>
-      <c r="G72">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A73" s="2" t="s">
+      <c r="F72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
         <v>121</v>
       </c>
-      <c r="B73" s="2" t="s">
+      <c r="B73" t="s">
         <v>125</v>
       </c>
-      <c r="C73" s="4">
+      <c r="C73" s="2">
         <v>45930</v>
       </c>
-      <c r="D73" s="7">
+      <c r="D73" s="4">
         <v>5</v>
       </c>
-      <c r="E73" s="2">
-        <v>1</v>
-      </c>
-      <c r="F73" s="2"/>
-      <c r="G73">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="E73">
+        <v>1</v>
+      </c>
+      <c r="F73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>122</v>
       </c>
       <c r="B74" t="s">
         <v>126</v>
       </c>
-      <c r="C74" s="3">
+      <c r="C74" s="2">
         <v>45931</v>
       </c>
-      <c r="D74" s="6">
+      <c r="D74" s="4">
         <v>5</v>
       </c>
       <c r="E74">
         <v>1</v>
       </c>
-      <c r="F74"/>
-      <c r="G74">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>127</v>
       </c>
       <c r="B75" t="s">
         <v>128</v>
       </c>
-      <c r="C75" s="3">
+      <c r="C75" s="2">
         <v>45932</v>
       </c>
-      <c r="D75" s="6">
+      <c r="D75" s="4">
         <v>5</v>
       </c>
       <c r="E75">
         <v>1</v>
       </c>
-      <c r="G75">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>129</v>
       </c>
       <c r="B76" t="s">
         <v>132</v>
       </c>
-      <c r="C76" s="3">
+      <c r="C76" s="2">
         <v>45932</v>
       </c>
-      <c r="D76" s="6">
+      <c r="D76" s="4">
         <v>5</v>
       </c>
       <c r="E76">
         <v>1</v>
       </c>
-      <c r="F76" t="s">
-        <v>199</v>
-      </c>
-      <c r="G76">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>130</v>
       </c>
       <c r="B77" t="s">
         <v>133</v>
       </c>
-      <c r="C77" s="3">
+      <c r="C77" s="2">
         <v>45932</v>
       </c>
-      <c r="D77" s="6">
+      <c r="D77" s="4">
         <v>5</v>
       </c>
       <c r="E77">
         <v>1</v>
       </c>
-      <c r="F77" t="s">
-        <v>199</v>
-      </c>
-      <c r="G77">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>131</v>
       </c>
       <c r="B78" t="s">
         <v>134</v>
       </c>
-      <c r="C78" s="3">
+      <c r="C78" s="2">
         <v>45932</v>
       </c>
-      <c r="D78" s="6">
+      <c r="D78" s="4">
         <v>5</v>
       </c>
       <c r="E78">
         <v>1</v>
       </c>
-      <c r="F78" t="s">
-        <v>199</v>
-      </c>
-      <c r="G78">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>166</v>
       </c>
       <c r="B79" t="s">
-        <v>203</v>
-      </c>
-      <c r="C79" s="3">
+        <v>201</v>
+      </c>
+      <c r="C79" s="2">
         <v>45933</v>
       </c>
-      <c r="D79" s="6">
+      <c r="D79" s="4">
         <v>5</v>
       </c>
       <c r="E79">
         <v>1</v>
       </c>
-      <c r="F79" t="s">
-        <v>199</v>
-      </c>
-      <c r="G79">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>135</v>
       </c>
       <c r="B80" t="s">
         <v>138</v>
       </c>
-      <c r="C80" s="3">
+      <c r="C80" s="2">
         <v>45934</v>
       </c>
-      <c r="D80" s="6">
+      <c r="D80" s="4">
         <v>5</v>
       </c>
       <c r="E80">
         <v>1</v>
       </c>
-      <c r="G80">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>136</v>
       </c>
       <c r="B81" t="s">
         <v>137</v>
       </c>
-      <c r="C81" s="3">
+      <c r="C81" s="2">
         <v>45934</v>
       </c>
-      <c r="D81" s="6">
+      <c r="D81" s="4">
         <v>5</v>
       </c>
       <c r="E81">
         <v>1</v>
       </c>
-      <c r="F81" t="s">
-        <v>199</v>
-      </c>
-      <c r="G81">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>141</v>
       </c>
       <c r="B82" t="s">
         <v>139</v>
       </c>
-      <c r="C82" s="3">
+      <c r="C82" s="2">
         <v>45936</v>
       </c>
-      <c r="D82" s="6">
+      <c r="D82" s="4">
         <v>6</v>
       </c>
       <c r="E82">
         <v>1</v>
       </c>
-      <c r="G82">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="F82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>140</v>
       </c>
       <c r="B83" t="s">
         <v>144</v>
       </c>
-      <c r="C83" s="3">
+      <c r="C83" s="2">
         <v>45936</v>
       </c>
-      <c r="D83" s="6">
+      <c r="D83" s="4">
         <v>6</v>
       </c>
       <c r="E83">
         <v>1</v>
       </c>
-      <c r="F83"/>
-      <c r="G83">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>142</v>
       </c>
       <c r="B84" t="s">
         <v>145</v>
       </c>
-      <c r="C84" s="3">
+      <c r="C84" s="2">
         <v>45936</v>
       </c>
-      <c r="D84" s="6">
+      <c r="D84" s="4">
         <v>6</v>
       </c>
       <c r="E84">
         <v>1</v>
       </c>
-      <c r="G84">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>143</v>
       </c>
       <c r="B85" t="s">
         <v>146</v>
       </c>
-      <c r="C85" s="3">
+      <c r="C85" s="2">
         <v>45936</v>
       </c>
-      <c r="D85" s="6">
+      <c r="D85" s="4">
         <v>6</v>
       </c>
       <c r="E85">
         <v>1</v>
       </c>
-      <c r="G85">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="F85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>148</v>
       </c>
       <c r="B86" t="s">
         <v>147</v>
       </c>
-      <c r="C86" s="3">
+      <c r="C86" s="2">
         <v>45937</v>
       </c>
-      <c r="D86" s="6">
+      <c r="D86" s="4">
         <v>6</v>
       </c>
       <c r="E86">
         <v>1</v>
       </c>
-      <c r="F86" t="s">
-        <v>199</v>
-      </c>
-      <c r="G86">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="F86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>149</v>
       </c>
       <c r="B87" t="s">
         <v>150</v>
       </c>
-      <c r="C87" s="3">
+      <c r="C87" s="2">
         <v>45938</v>
       </c>
-      <c r="D87" s="6">
+      <c r="D87" s="4">
         <v>6</v>
       </c>
       <c r="E87">
         <v>1</v>
       </c>
-      <c r="F87"/>
-      <c r="G87">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A88" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="B88" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="C88" s="4">
+      <c r="F87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>224</v>
+      </c>
+      <c r="B88" t="s">
+        <v>225</v>
+      </c>
+      <c r="C88" s="2">
         <v>45938</v>
       </c>
-      <c r="D88" s="7">
+      <c r="D88" s="4">
         <v>6</v>
       </c>
-      <c r="E88" s="2">
-        <v>1</v>
-      </c>
-      <c r="F88" s="2"/>
-      <c r="G88">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E88">
+        <v>1</v>
+      </c>
+      <c r="F88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>151</v>
       </c>
       <c r="B89" t="s">
         <v>152</v>
       </c>
-      <c r="C89" s="3">
+      <c r="C89" s="2">
         <v>45938</v>
       </c>
-      <c r="D89" s="6">
+      <c r="D89" s="4">
         <v>6</v>
       </c>
       <c r="E89">
         <v>1</v>
       </c>
-      <c r="G89">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>153</v>
       </c>
       <c r="B90" t="s">
         <v>159</v>
       </c>
-      <c r="C90" s="3">
+      <c r="C90" s="2">
         <v>45939</v>
       </c>
-      <c r="D90" s="6">
+      <c r="D90" s="4">
         <v>6</v>
       </c>
       <c r="E90">
         <v>1</v>
       </c>
-      <c r="F90" t="s">
-        <v>199</v>
-      </c>
-      <c r="G90">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>154</v>
       </c>
       <c r="B91" t="s">
         <v>160</v>
       </c>
-      <c r="C91" s="3">
+      <c r="C91" s="2">
         <v>45939</v>
       </c>
-      <c r="D91" s="6">
+      <c r="D91" s="4">
         <v>6</v>
       </c>
       <c r="E91">
         <v>1</v>
       </c>
-      <c r="F91" t="s">
-        <v>199</v>
-      </c>
-      <c r="G91">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>155</v>
       </c>
       <c r="B92" t="s">
         <v>161</v>
       </c>
-      <c r="C92" s="3">
+      <c r="C92" s="2">
         <v>45939</v>
       </c>
-      <c r="D92" s="6">
+      <c r="D92" s="4">
         <v>6</v>
       </c>
       <c r="E92">
         <v>1</v>
       </c>
-      <c r="G92">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>156</v>
       </c>
       <c r="B93" t="s">
         <v>162</v>
       </c>
-      <c r="C93" s="3">
+      <c r="C93" s="2">
         <v>45939</v>
       </c>
-      <c r="D93" s="6">
+      <c r="D93" s="4">
         <v>6</v>
       </c>
       <c r="E93">
         <v>1</v>
       </c>
-      <c r="F93" t="s">
-        <v>199</v>
-      </c>
-      <c r="G93">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>157</v>
       </c>
       <c r="B94" t="s">
         <v>163</v>
       </c>
-      <c r="C94" s="3">
+      <c r="C94" s="2">
         <v>45939</v>
       </c>
-      <c r="D94" s="6">
+      <c r="D94" s="4">
         <v>6</v>
       </c>
       <c r="E94">
         <v>1</v>
       </c>
-      <c r="G94">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>158</v>
       </c>
       <c r="B95" t="s">
         <v>164</v>
       </c>
-      <c r="C95" s="3">
+      <c r="C95" s="2">
         <v>45939</v>
       </c>
-      <c r="D95" s="6">
+      <c r="D95" s="4">
         <v>6</v>
       </c>
       <c r="E95">
         <v>1</v>
       </c>
-      <c r="G95">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>165</v>
       </c>
       <c r="B96" t="s">
         <v>167</v>
       </c>
-      <c r="C96" s="3">
+      <c r="C96" s="2">
         <v>45941</v>
       </c>
-      <c r="D96" s="6">
+      <c r="D96" s="4">
         <v>6</v>
       </c>
       <c r="E96">
         <v>1</v>
       </c>
-      <c r="G96">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="97" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="F96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>170</v>
       </c>
       <c r="B97" t="s">
         <v>180</v>
       </c>
-      <c r="C97" s="3">
+      <c r="C97" s="2">
         <v>45945</v>
       </c>
-      <c r="D97" s="6">
+      <c r="D97" s="4">
         <v>7</v>
       </c>
       <c r="E97">
         <v>1</v>
       </c>
-      <c r="F97"/>
-      <c r="G97">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>175</v>
       </c>
       <c r="B98" t="s">
         <v>185</v>
       </c>
-      <c r="C98" s="3">
+      <c r="C98" s="2">
         <v>45945</v>
       </c>
-      <c r="D98" s="6">
+      <c r="D98" s="4">
         <v>7</v>
       </c>
       <c r="E98">
         <v>1</v>
       </c>
-      <c r="G98">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>171</v>
       </c>
       <c r="B99" t="s">
         <v>181</v>
       </c>
-      <c r="C99" s="3">
+      <c r="C99" s="2">
         <v>45945</v>
       </c>
-      <c r="D99" s="6">
+      <c r="D99" s="4">
         <v>7</v>
       </c>
       <c r="E99">
         <v>1</v>
       </c>
-      <c r="G99">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>176</v>
       </c>
       <c r="B100" t="s">
         <v>186</v>
       </c>
-      <c r="C100" s="3">
+      <c r="C100" s="2">
         <v>45945</v>
       </c>
-      <c r="D100" s="6">
+      <c r="D100" s="4">
         <v>7</v>
       </c>
       <c r="E100">
         <v>1</v>
       </c>
-      <c r="F100" t="s">
-        <v>199</v>
-      </c>
-      <c r="G100">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F100">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>177</v>
       </c>
       <c r="B101" t="s">
         <v>187</v>
       </c>
-      <c r="C101" s="3">
+      <c r="C101" s="2">
         <v>45945</v>
       </c>
-      <c r="D101" s="6">
+      <c r="D101" s="4">
         <v>7</v>
       </c>
       <c r="E101">
         <v>1</v>
       </c>
-      <c r="G101">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>178</v>
       </c>
       <c r="B102" t="s">
         <v>188</v>
       </c>
-      <c r="C102" s="3">
+      <c r="C102" s="2">
         <v>45945</v>
       </c>
-      <c r="D102" s="6">
+      <c r="D102" s="4">
         <v>7</v>
       </c>
       <c r="E102">
         <v>1</v>
       </c>
-      <c r="G102">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F102">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>179</v>
       </c>
       <c r="B103" t="s">
         <v>189</v>
       </c>
-      <c r="C103" s="3">
+      <c r="C103" s="2">
         <v>45945</v>
       </c>
-      <c r="D103" s="6">
+      <c r="D103" s="4">
         <v>7</v>
       </c>
       <c r="E103">
         <v>1</v>
       </c>
-      <c r="F103" t="s">
-        <v>199</v>
-      </c>
-      <c r="G103">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F103">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
         <v>190</v>
       </c>
       <c r="B104" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="C104" s="5">
+      <c r="C104" s="3">
         <v>45946</v>
       </c>
-      <c r="D104" s="8">
+      <c r="D104" s="5">
         <v>7</v>
       </c>
       <c r="E104" s="1">
         <v>1</v>
       </c>
-      <c r="F104" s="1"/>
-      <c r="G104">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="105" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A105" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="B105" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="C105" s="4">
+      <c r="F104">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>226</v>
+      </c>
+      <c r="B105" t="s">
+        <v>227</v>
+      </c>
+      <c r="C105" s="2">
         <v>45946</v>
       </c>
-      <c r="D105" s="7">
+      <c r="D105" s="4">
         <v>7</v>
       </c>
-      <c r="E105" s="2">
-        <v>1</v>
-      </c>
-      <c r="G105">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A106" s="2" t="s">
+      <c r="E105">
+        <v>1</v>
+      </c>
+      <c r="F105">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
         <v>168</v>
       </c>
-      <c r="B106" s="2" t="s">
+      <c r="B106" t="s">
         <v>169</v>
       </c>
-      <c r="C106" s="4">
+      <c r="C106" s="2">
         <v>45946</v>
       </c>
-      <c r="D106" s="7">
+      <c r="D106" s="4">
         <v>7</v>
       </c>
-      <c r="E106" s="2">
-        <v>1</v>
-      </c>
-      <c r="F106" s="2"/>
-      <c r="G106">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E106">
+        <v>1</v>
+      </c>
+      <c r="F106">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>172</v>
       </c>
       <c r="B107" t="s">
         <v>182</v>
       </c>
-      <c r="C107" s="3">
+      <c r="C107" s="2">
         <v>45946</v>
       </c>
-      <c r="D107" s="6">
+      <c r="D107" s="4">
         <v>7</v>
       </c>
       <c r="E107">
         <v>1</v>
       </c>
-      <c r="F107" t="s">
-        <v>199</v>
-      </c>
-      <c r="G107">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="108" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="F107">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>173</v>
       </c>
       <c r="B108" t="s">
         <v>183</v>
       </c>
-      <c r="C108" s="3">
+      <c r="C108" s="2">
         <v>45946</v>
       </c>
-      <c r="D108" s="6">
+      <c r="D108" s="4">
         <v>7</v>
       </c>
       <c r="E108">
         <v>1</v>
       </c>
-      <c r="F108"/>
-      <c r="G108">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="109" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="F108">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>174</v>
       </c>
       <c r="B109" t="s">
         <v>184</v>
       </c>
-      <c r="C109" s="3">
+      <c r="C109" s="2">
         <v>45946</v>
       </c>
-      <c r="D109" s="6">
+      <c r="D109" s="4">
         <v>7</v>
       </c>
       <c r="E109">
         <v>1</v>
       </c>
-      <c r="F109"/>
-      <c r="G109">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>193</v>
       </c>
       <c r="B110" t="s">
         <v>196</v>
       </c>
-      <c r="C110" s="3">
+      <c r="C110" s="2">
         <v>45955</v>
       </c>
-      <c r="D110" s="6">
+      <c r="D110" s="4">
         <v>8</v>
       </c>
       <c r="E110">
         <v>1</v>
       </c>
-      <c r="F110" t="s">
-        <v>199</v>
-      </c>
-      <c r="G110">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>192</v>
       </c>
       <c r="B111" t="s">
         <v>195</v>
       </c>
-      <c r="C111" s="3">
+      <c r="C111" s="2">
         <v>45955</v>
       </c>
-      <c r="D111" s="6">
+      <c r="D111" s="4">
         <v>8</v>
       </c>
       <c r="E111">
         <v>1</v>
       </c>
-      <c r="F111" t="s">
-        <v>199</v>
-      </c>
-      <c r="G111">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F111">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>194</v>
       </c>
       <c r="B112" t="s">
         <v>197</v>
       </c>
-      <c r="C112" s="3">
+      <c r="C112" s="2">
         <v>228576</v>
       </c>
-      <c r="D112" s="6">
+      <c r="D112" s="4">
         <v>8</v>
       </c>
       <c r="E112">
         <v>1</v>
       </c>
-      <c r="F112" t="s">
-        <v>199</v>
-      </c>
-      <c r="G112">
+      <c r="F112">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G121">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F121">
     <sortCondition ref="C2:C121"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Finish out week 3 data
</commit_message>
<xml_diff>
--- a/2025/meet_list_data_ready.xlsx
+++ b/2025/meet_list_data_ready.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dburk\Documents\GitHub\sdxc-data\2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67752897-B593-4CA9-9906-17B8F71D9B60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98FC79B0-E4B7-4373-ADB6-4B528FDAEC02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1EB159B1-87E3-4E73-9839-0175057112CF}"/>
+    <workbookView xWindow="2268" yWindow="1560" windowWidth="17280" windowHeight="10680" xr2:uid="{1EB159B1-87E3-4E73-9839-0175057112CF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1104,8 +1104,8 @@
   <dimension ref="A1:F108"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K31" sqref="K31"/>
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2033,7 +2033,7 @@
         <v>1</v>
       </c>
       <c r="F46">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>